<commit_message>
Adding NDMA pilot pages, adding NDVI monitoring, late NOV data update
</commit_message>
<xml_diff>
--- a/passage_clusters/VIIRS/CLUSTER_1/VCI3M_Forecast_Overview_CLUSTER_1.xlsx
+++ b/passage_clusters/VIIRS/CLUSTER_1/VCI3M_Forecast_Overview_CLUSTER_1.xlsx
@@ -445,37 +445,37 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="B1" s="1">
-        <v>45606</v>
+        <v>45613</v>
       </c>
       <c r="C1" s="1">
-        <v>45613</v>
+        <v>45620</v>
       </c>
       <c r="D1" s="1">
-        <v>45620</v>
+        <v>45627</v>
       </c>
       <c r="E1" s="1">
-        <v>45627</v>
+        <v>45634</v>
       </c>
       <c r="F1" s="1">
-        <v>45634</v>
+        <v>45641</v>
       </c>
       <c r="G1" s="1">
-        <v>45641</v>
+        <v>45648</v>
       </c>
       <c r="H1" s="1">
-        <v>45648</v>
+        <v>45655</v>
       </c>
       <c r="I1" s="1">
-        <v>45655</v>
+        <v>45662</v>
       </c>
       <c r="J1" s="1">
-        <v>45662</v>
+        <v>45669</v>
       </c>
       <c r="K1" s="1">
-        <v>45669</v>
+        <v>45676</v>
       </c>
       <c r="L1" s="1">
-        <v>45676</v>
+        <v>45683</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -483,37 +483,37 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>73.8</v>
+        <v>72.90000000000001</v>
       </c>
       <c r="C2">
-        <v>72.90000000000001</v>
+        <v>71.59999999999999</v>
       </c>
       <c r="D2">
-        <v>71.59999999999999</v>
+        <v>70.09999999999999</v>
       </c>
       <c r="E2">
-        <v>70.09999999999999</v>
+        <v>68.59999999999999</v>
       </c>
       <c r="F2">
-        <v>68.5</v>
+        <v>67</v>
       </c>
       <c r="G2">
-        <v>66.90000000000001</v>
+        <v>65.59999999999999</v>
       </c>
       <c r="H2">
-        <v>65.5</v>
+        <v>64.3</v>
       </c>
       <c r="I2">
-        <v>64.09999999999999</v>
+        <v>63.1</v>
       </c>
       <c r="J2">
-        <v>62.9</v>
+        <v>62</v>
       </c>
       <c r="K2">
-        <v>61.8</v>
+        <v>61</v>
       </c>
       <c r="L2">
-        <v>60.7</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -521,37 +521,37 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>51.9</v>
+        <v>52.7</v>
       </c>
       <c r="C3">
-        <v>52.6</v>
+        <v>53.1</v>
       </c>
       <c r="D3">
-        <v>52.8</v>
+        <v>53</v>
       </c>
       <c r="E3">
         <v>52.4</v>
       </c>
       <c r="F3">
-        <v>51.5</v>
+        <v>51.4</v>
       </c>
       <c r="G3">
         <v>50.1</v>
       </c>
       <c r="H3">
-        <v>48.2</v>
+        <v>48.5</v>
       </c>
       <c r="I3">
-        <v>46.2</v>
+        <v>46.9</v>
       </c>
       <c r="J3">
-        <v>43.9</v>
+        <v>45.2</v>
       </c>
       <c r="K3">
-        <v>41.7</v>
+        <v>43.7</v>
       </c>
       <c r="L3">
-        <v>39.7</v>
+        <v>42.4</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -559,37 +559,37 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>53.5</v>
+        <v>53.2</v>
       </c>
       <c r="C4">
-        <v>53.1</v>
+        <v>52.5</v>
       </c>
       <c r="D4">
-        <v>52.3</v>
+        <v>51.4</v>
       </c>
       <c r="E4">
-        <v>51.1</v>
+        <v>50.1</v>
       </c>
       <c r="F4">
-        <v>49.6</v>
+        <v>48.7</v>
       </c>
       <c r="G4">
-        <v>48</v>
+        <v>47.3</v>
       </c>
       <c r="H4">
-        <v>46.4</v>
+        <v>46</v>
       </c>
       <c r="I4">
-        <v>44.8</v>
+        <v>44.7</v>
       </c>
       <c r="J4">
-        <v>43.3</v>
+        <v>43.6</v>
       </c>
       <c r="K4">
+        <v>42.7</v>
+      </c>
+      <c r="L4">
         <v>41.9</v>
-      </c>
-      <c r="L4">
-        <v>40.7</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -597,37 +597,37 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>73.3</v>
+        <v>74.09999999999999</v>
       </c>
       <c r="C5">
-        <v>74.09999999999999</v>
+        <v>74.40000000000001</v>
       </c>
       <c r="D5">
         <v>74.40000000000001</v>
       </c>
       <c r="E5">
-        <v>74.40000000000001</v>
+        <v>74.09999999999999</v>
       </c>
       <c r="F5">
-        <v>74.09999999999999</v>
+        <v>73.59999999999999</v>
       </c>
       <c r="G5">
-        <v>73.5</v>
+        <v>72.90000000000001</v>
       </c>
       <c r="H5">
-        <v>72.8</v>
+        <v>72.2</v>
       </c>
       <c r="I5">
-        <v>72</v>
+        <v>71.3</v>
       </c>
       <c r="J5">
-        <v>71.09999999999999</v>
+        <v>70.40000000000001</v>
       </c>
       <c r="K5">
-        <v>70.09999999999999</v>
+        <v>69.5</v>
       </c>
       <c r="L5">
-        <v>69.2</v>
+        <v>68.5</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -635,37 +635,37 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>74.2</v>
+        <v>69.59999999999999</v>
       </c>
       <c r="C6">
-        <v>69.3</v>
+        <v>64.90000000000001</v>
       </c>
       <c r="D6">
-        <v>64</v>
+        <v>60.1</v>
       </c>
       <c r="E6">
-        <v>58.6</v>
+        <v>55.4</v>
       </c>
       <c r="F6">
-        <v>53.1</v>
+        <v>51.1</v>
       </c>
       <c r="G6">
-        <v>47.7</v>
+        <v>47.1</v>
       </c>
       <c r="H6">
-        <v>42.5</v>
+        <v>43.6</v>
       </c>
       <c r="I6">
-        <v>37.6</v>
+        <v>40.7</v>
       </c>
       <c r="J6">
-        <v>33.3</v>
+        <v>38.3</v>
       </c>
       <c r="K6">
-        <v>29.5</v>
+        <v>36.5</v>
       </c>
       <c r="L6">
-        <v>26.4</v>
+        <v>35.4</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -673,37 +673,37 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>80.5</v>
+        <v>76.5</v>
       </c>
       <c r="C7">
-        <v>76.90000000000001</v>
+        <v>72.59999999999999</v>
       </c>
       <c r="D7">
-        <v>73.5</v>
+        <v>68.8</v>
       </c>
       <c r="E7">
-        <v>70.3</v>
+        <v>65.3</v>
       </c>
       <c r="F7">
-        <v>67.7</v>
+        <v>62.2</v>
       </c>
       <c r="G7">
-        <v>65.7</v>
+        <v>59.4</v>
       </c>
       <c r="H7">
-        <v>64.09999999999999</v>
+        <v>56.8</v>
       </c>
       <c r="I7">
-        <v>62.9</v>
+        <v>54.4</v>
       </c>
       <c r="J7">
-        <v>62</v>
+        <v>52.1</v>
       </c>
       <c r="K7">
-        <v>61</v>
+        <v>49.7</v>
       </c>
       <c r="L7">
-        <v>60</v>
+        <v>47.2</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -711,37 +711,37 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>79.90000000000001</v>
+        <v>80.7</v>
       </c>
       <c r="C8">
+        <v>80.90000000000001</v>
+      </c>
+      <c r="D8">
+        <v>80.8</v>
+      </c>
+      <c r="E8">
         <v>80.5</v>
       </c>
-      <c r="D8">
-        <v>80.5</v>
-      </c>
-      <c r="E8">
-        <v>80</v>
-      </c>
       <c r="F8">
+        <v>80.09999999999999</v>
+      </c>
+      <c r="G8">
+        <v>79.7</v>
+      </c>
+      <c r="H8">
+        <v>79.5</v>
+      </c>
+      <c r="I8">
+        <v>79.40000000000001</v>
+      </c>
+      <c r="J8">
+        <v>79.40000000000001</v>
+      </c>
+      <c r="K8">
+        <v>79.3</v>
+      </c>
+      <c r="L8">
         <v>79.2</v>
-      </c>
-      <c r="G8">
-        <v>78.2</v>
-      </c>
-      <c r="H8">
-        <v>77.2</v>
-      </c>
-      <c r="I8">
-        <v>76.2</v>
-      </c>
-      <c r="J8">
-        <v>75.40000000000001</v>
-      </c>
-      <c r="K8">
-        <v>74.59999999999999</v>
-      </c>
-      <c r="L8">
-        <v>73.8</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -749,37 +749,37 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>79</v>
+        <v>78.7</v>
       </c>
       <c r="C9">
-        <v>78.90000000000001</v>
+        <v>78.09999999999999</v>
       </c>
       <c r="D9">
-        <v>78.59999999999999</v>
+        <v>77.40000000000001</v>
       </c>
       <c r="E9">
-        <v>78.3</v>
+        <v>76.7</v>
       </c>
       <c r="F9">
-        <v>78.09999999999999</v>
+        <v>76.09999999999999</v>
       </c>
       <c r="G9">
-        <v>78.2</v>
+        <v>75.7</v>
       </c>
       <c r="H9">
-        <v>78.5</v>
+        <v>75.5</v>
       </c>
       <c r="I9">
-        <v>79</v>
+        <v>75.2</v>
       </c>
       <c r="J9">
-        <v>79.59999999999999</v>
+        <v>74.90000000000001</v>
       </c>
       <c r="K9">
-        <v>80.09999999999999</v>
+        <v>74.40000000000001</v>
       </c>
       <c r="L9">
-        <v>80.40000000000001</v>
+        <v>73.59999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -787,37 +787,37 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>78.8</v>
+        <v>79.8</v>
       </c>
       <c r="C10">
         <v>80</v>
       </c>
       <c r="D10">
-        <v>80.40000000000001</v>
+        <v>79.40000000000001</v>
       </c>
       <c r="E10">
-        <v>80.09999999999999</v>
+        <v>78</v>
       </c>
       <c r="F10">
-        <v>79.09999999999999</v>
+        <v>75.90000000000001</v>
       </c>
       <c r="G10">
-        <v>77.5</v>
+        <v>73.2</v>
       </c>
       <c r="H10">
-        <v>75.40000000000001</v>
+        <v>70.09999999999999</v>
       </c>
       <c r="I10">
-        <v>72.90000000000001</v>
+        <v>66.7</v>
       </c>
       <c r="J10">
-        <v>70.2</v>
+        <v>63.2</v>
       </c>
       <c r="K10">
-        <v>67.3</v>
+        <v>59.6</v>
       </c>
       <c r="L10">
-        <v>64.3</v>
+        <v>56.1</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -825,37 +825,37 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>84.7</v>
+        <v>85.2</v>
       </c>
       <c r="C11">
-        <v>85.2</v>
+        <v>85.3</v>
       </c>
       <c r="D11">
         <v>85.3</v>
       </c>
       <c r="E11">
-        <v>85.2</v>
+        <v>85.09999999999999</v>
       </c>
       <c r="F11">
-        <v>85</v>
+        <v>84.90000000000001</v>
       </c>
       <c r="G11">
         <v>84.7</v>
       </c>
       <c r="H11">
-        <v>84.40000000000001</v>
+        <v>84.3</v>
       </c>
       <c r="I11">
-        <v>83.90000000000001</v>
+        <v>83.8</v>
       </c>
       <c r="J11">
-        <v>83.40000000000001</v>
+        <v>83.2</v>
       </c>
       <c r="K11">
-        <v>82.59999999999999</v>
+        <v>82.2</v>
       </c>
       <c r="L11">
-        <v>81.59999999999999</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -863,28 +863,28 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>69.3</v>
+        <v>70.8</v>
       </c>
       <c r="C12">
-        <v>70.8</v>
+        <v>71.8</v>
       </c>
       <c r="D12">
-        <v>71.7</v>
+        <v>72.3</v>
       </c>
       <c r="E12">
-        <v>72.2</v>
+        <v>72.40000000000001</v>
       </c>
       <c r="F12">
         <v>72.2</v>
       </c>
       <c r="G12">
-        <v>71.90000000000001</v>
+        <v>71.8</v>
       </c>
       <c r="H12">
-        <v>71.40000000000001</v>
+        <v>71.2</v>
       </c>
       <c r="I12">
-        <v>70.7</v>
+        <v>70.5</v>
       </c>
       <c r="J12">
         <v>69.8</v>
@@ -901,37 +901,37 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>68.3</v>
+        <v>68.90000000000001</v>
       </c>
       <c r="C13">
-        <v>68.8</v>
+        <v>68.90000000000001</v>
       </c>
       <c r="D13">
-        <v>68.7</v>
+        <v>68.5</v>
       </c>
       <c r="E13">
-        <v>68.2</v>
+        <v>67.7</v>
       </c>
       <c r="F13">
-        <v>67.2</v>
+        <v>66.5</v>
       </c>
       <c r="G13">
-        <v>65.7</v>
+        <v>65</v>
       </c>
       <c r="H13">
-        <v>63.9</v>
+        <v>63.3</v>
       </c>
       <c r="I13">
-        <v>61.9</v>
+        <v>61.4</v>
       </c>
       <c r="J13">
-        <v>59.7</v>
+        <v>59.4</v>
       </c>
       <c r="K13">
-        <v>57.3</v>
+        <v>57.4</v>
       </c>
       <c r="L13">
-        <v>55</v>
+        <v>55.4</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -939,37 +939,37 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>89.7</v>
+        <v>85.59999999999999</v>
       </c>
       <c r="C14">
-        <v>85.5</v>
+        <v>81.09999999999999</v>
       </c>
       <c r="D14">
-        <v>80.90000000000001</v>
+        <v>76.90000000000001</v>
       </c>
       <c r="E14">
-        <v>76.5</v>
+        <v>73</v>
       </c>
       <c r="F14">
-        <v>72.5</v>
+        <v>69.90000000000001</v>
       </c>
       <c r="G14">
-        <v>69.2</v>
+        <v>67.7</v>
       </c>
       <c r="H14">
-        <v>66.7</v>
+        <v>66.3</v>
       </c>
       <c r="I14">
-        <v>65</v>
+        <v>65.59999999999999</v>
       </c>
       <c r="J14">
-        <v>64</v>
+        <v>65.59999999999999</v>
       </c>
       <c r="K14">
-        <v>63.7</v>
+        <v>66</v>
       </c>
       <c r="L14">
-        <v>63.8</v>
+        <v>66.59999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -977,22 +977,22 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>80.09999999999999</v>
+        <v>79.40000000000001</v>
       </c>
       <c r="C15">
-        <v>79.40000000000001</v>
+        <v>78.7</v>
       </c>
       <c r="D15">
-        <v>78.8</v>
+        <v>78.09999999999999</v>
       </c>
       <c r="E15">
-        <v>78.2</v>
+        <v>77.8</v>
       </c>
       <c r="F15">
+        <v>77.8</v>
+      </c>
+      <c r="G15">
         <v>78</v>
-      </c>
-      <c r="G15">
-        <v>78.09999999999999</v>
       </c>
       <c r="H15">
         <v>78.5</v>
@@ -1001,13 +1001,13 @@
         <v>79.09999999999999</v>
       </c>
       <c r="J15">
-        <v>79.8</v>
+        <v>79.5</v>
       </c>
       <c r="K15">
-        <v>80.40000000000001</v>
+        <v>79.7</v>
       </c>
       <c r="L15">
-        <v>80.7</v>
+        <v>79.5</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1015,37 +1015,37 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>63.7</v>
+        <v>63.6</v>
       </c>
       <c r="C16">
-        <v>63.5</v>
+        <v>63.1</v>
       </c>
       <c r="D16">
-        <v>62.8</v>
+        <v>62.3</v>
       </c>
       <c r="E16">
-        <v>61.7</v>
+        <v>61.1</v>
       </c>
       <c r="F16">
-        <v>60.2</v>
+        <v>59.6</v>
       </c>
       <c r="G16">
-        <v>58.3</v>
+        <v>57.9</v>
       </c>
       <c r="H16">
-        <v>56.2</v>
+        <v>56.1</v>
       </c>
       <c r="I16">
-        <v>53.9</v>
+        <v>54.3</v>
       </c>
       <c r="J16">
-        <v>51.5</v>
+        <v>52.5</v>
       </c>
       <c r="K16">
-        <v>49.2</v>
+        <v>50.9</v>
       </c>
       <c r="L16">
-        <v>47</v>
+        <v>49.4</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1053,37 +1053,37 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>69.59999999999999</v>
+        <v>69.7</v>
       </c>
       <c r="C17">
-        <v>69.59999999999999</v>
+        <v>69.40000000000001</v>
       </c>
       <c r="D17">
-        <v>69.09999999999999</v>
+        <v>68.7</v>
       </c>
       <c r="E17">
-        <v>68.3</v>
+        <v>67.8</v>
       </c>
       <c r="F17">
-        <v>67.09999999999999</v>
+        <v>66.59999999999999</v>
       </c>
       <c r="G17">
-        <v>65.59999999999999</v>
+        <v>65.40000000000001</v>
       </c>
       <c r="H17">
-        <v>64</v>
+        <v>64.09999999999999</v>
       </c>
       <c r="I17">
-        <v>62.3</v>
+        <v>62.8</v>
       </c>
       <c r="J17">
-        <v>60.6</v>
+        <v>61.6</v>
       </c>
       <c r="K17">
-        <v>59</v>
+        <v>60.4</v>
       </c>
       <c r="L17">
-        <v>57.4</v>
+        <v>59.3</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1091,37 +1091,37 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>73.90000000000001</v>
+        <v>74.40000000000001</v>
       </c>
       <c r="C18">
+        <v>74.59999999999999</v>
+      </c>
+      <c r="D18">
+        <v>74.7</v>
+      </c>
+      <c r="E18">
+        <v>74.7</v>
+      </c>
+      <c r="F18">
+        <v>74.7</v>
+      </c>
+      <c r="G18">
+        <v>74.7</v>
+      </c>
+      <c r="H18">
+        <v>74.7</v>
+      </c>
+      <c r="I18">
+        <v>74.7</v>
+      </c>
+      <c r="J18">
         <v>74.5</v>
       </c>
-      <c r="D18">
-        <v>74.90000000000001</v>
-      </c>
-      <c r="E18">
-        <v>75.2</v>
-      </c>
-      <c r="F18">
-        <v>75.5</v>
-      </c>
-      <c r="G18">
-        <v>75.90000000000001</v>
-      </c>
-      <c r="H18">
-        <v>76.40000000000001</v>
-      </c>
-      <c r="I18">
-        <v>76.90000000000001</v>
-      </c>
-      <c r="J18">
-        <v>77.3</v>
-      </c>
       <c r="K18">
-        <v>77.7</v>
+        <v>74.09999999999999</v>
       </c>
       <c r="L18">
-        <v>77.8</v>
+        <v>73.5</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1129,37 +1129,37 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>77.8</v>
+        <v>73.3</v>
       </c>
       <c r="C19">
-        <v>73.3</v>
+        <v>68.3</v>
       </c>
       <c r="D19">
-        <v>68.40000000000001</v>
+        <v>63.3</v>
       </c>
       <c r="E19">
-        <v>63.5</v>
+        <v>58.5</v>
       </c>
       <c r="F19">
-        <v>58.9</v>
+        <v>54.2</v>
       </c>
       <c r="G19">
-        <v>54.8</v>
+        <v>50.6</v>
       </c>
       <c r="H19">
-        <v>51.4</v>
+        <v>47.5</v>
       </c>
       <c r="I19">
-        <v>48.6</v>
+        <v>45.2</v>
       </c>
       <c r="J19">
-        <v>46.5</v>
+        <v>43.4</v>
       </c>
       <c r="K19">
-        <v>44.9</v>
+        <v>42.1</v>
       </c>
       <c r="L19">
-        <v>43.9</v>
+        <v>41.3</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1167,37 +1167,37 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>83.59999999999999</v>
+        <v>79.5</v>
       </c>
       <c r="C20">
-        <v>79.59999999999999</v>
+        <v>75.59999999999999</v>
       </c>
       <c r="D20">
-        <v>75.8</v>
+        <v>72.3</v>
       </c>
       <c r="E20">
-        <v>72.59999999999999</v>
+        <v>69.8</v>
       </c>
       <c r="F20">
-        <v>70.3</v>
+        <v>68.2</v>
       </c>
       <c r="G20">
-        <v>69</v>
+        <v>67.59999999999999</v>
       </c>
       <c r="H20">
-        <v>68.7</v>
+        <v>67.8</v>
       </c>
       <c r="I20">
-        <v>69.3</v>
+        <v>68.59999999999999</v>
       </c>
       <c r="J20">
-        <v>70.40000000000001</v>
+        <v>69.59999999999999</v>
       </c>
       <c r="K20">
-        <v>71.7</v>
+        <v>70.59999999999999</v>
       </c>
       <c r="L20">
-        <v>73</v>
+        <v>71.3</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1205,37 +1205,37 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>70.90000000000001</v>
+        <v>69.3</v>
       </c>
       <c r="C21">
-        <v>69.3</v>
+        <v>67.2</v>
       </c>
       <c r="D21">
-        <v>67.2</v>
+        <v>64.8</v>
       </c>
       <c r="E21">
-        <v>64.7</v>
+        <v>62.2</v>
       </c>
       <c r="F21">
-        <v>62.2</v>
+        <v>59.7</v>
       </c>
       <c r="G21">
-        <v>59.6</v>
+        <v>57.4</v>
       </c>
       <c r="H21">
-        <v>57.3</v>
+        <v>55.3</v>
       </c>
       <c r="I21">
-        <v>55.2</v>
+        <v>53.6</v>
       </c>
       <c r="J21">
-        <v>53.4</v>
+        <v>52.1</v>
       </c>
       <c r="K21">
-        <v>51.9</v>
+        <v>51</v>
       </c>
       <c r="L21">
-        <v>50.7</v>
+        <v>50.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating data for december
</commit_message>
<xml_diff>
--- a/passage_clusters/VIIRS/CLUSTER_1/VCI3M_Forecast_Overview_CLUSTER_1.xlsx
+++ b/passage_clusters/VIIRS/CLUSTER_1/VCI3M_Forecast_Overview_CLUSTER_1.xlsx
@@ -445,37 +445,37 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="B1" s="1">
-        <v>45613</v>
+        <v>45627</v>
       </c>
       <c r="C1" s="1">
-        <v>45620</v>
+        <v>45634</v>
       </c>
       <c r="D1" s="1">
-        <v>45627</v>
+        <v>45641</v>
       </c>
       <c r="E1" s="1">
-        <v>45634</v>
+        <v>45648</v>
       </c>
       <c r="F1" s="1">
-        <v>45641</v>
+        <v>45655</v>
       </c>
       <c r="G1" s="1">
-        <v>45648</v>
+        <v>45662</v>
       </c>
       <c r="H1" s="1">
-        <v>45655</v>
+        <v>45669</v>
       </c>
       <c r="I1" s="1">
-        <v>45662</v>
+        <v>45676</v>
       </c>
       <c r="J1" s="1">
-        <v>45669</v>
+        <v>45683</v>
       </c>
       <c r="K1" s="1">
-        <v>45676</v>
+        <v>45690</v>
       </c>
       <c r="L1" s="1">
-        <v>45683</v>
+        <v>45697</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -483,37 +483,37 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>72.90000000000001</v>
+        <v>70.59999999999999</v>
       </c>
       <c r="C2">
-        <v>71.59999999999999</v>
+        <v>69.5</v>
       </c>
       <c r="D2">
-        <v>70.09999999999999</v>
+        <v>68.59999999999999</v>
       </c>
       <c r="E2">
-        <v>68.59999999999999</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="F2">
-        <v>67</v>
+        <v>67.5</v>
       </c>
       <c r="G2">
-        <v>65.59999999999999</v>
+        <v>67.3</v>
       </c>
       <c r="H2">
-        <v>64.3</v>
+        <v>67.2</v>
       </c>
       <c r="I2">
-        <v>63.1</v>
+        <v>67.2</v>
       </c>
       <c r="J2">
-        <v>62</v>
+        <v>67.3</v>
       </c>
       <c r="K2">
-        <v>61</v>
+        <v>67.2</v>
       </c>
       <c r="L2">
-        <v>60</v>
+        <v>66.90000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -521,37 +521,37 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>52.7</v>
+        <v>54.9</v>
       </c>
       <c r="C3">
-        <v>53.1</v>
+        <v>55.9</v>
       </c>
       <c r="D3">
-        <v>53</v>
+        <v>57.2</v>
       </c>
       <c r="E3">
-        <v>52.4</v>
+        <v>58.7</v>
       </c>
       <c r="F3">
-        <v>51.4</v>
+        <v>60.6</v>
       </c>
       <c r="G3">
-        <v>50.1</v>
+        <v>62.7</v>
       </c>
       <c r="H3">
-        <v>48.5</v>
+        <v>65.09999999999999</v>
       </c>
       <c r="I3">
-        <v>46.9</v>
+        <v>67.7</v>
       </c>
       <c r="J3">
-        <v>45.2</v>
+        <v>70.40000000000001</v>
       </c>
       <c r="K3">
-        <v>43.7</v>
+        <v>72.90000000000001</v>
       </c>
       <c r="L3">
-        <v>42.4</v>
+        <v>75.2</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -559,37 +559,37 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>53.2</v>
+        <v>51.9</v>
       </c>
       <c r="C4">
-        <v>52.5</v>
+        <v>51.1</v>
       </c>
       <c r="D4">
-        <v>51.4</v>
+        <v>50.3</v>
       </c>
       <c r="E4">
-        <v>50.1</v>
+        <v>49.7</v>
       </c>
       <c r="F4">
-        <v>48.7</v>
+        <v>49.3</v>
       </c>
       <c r="G4">
-        <v>47.3</v>
+        <v>49.2</v>
       </c>
       <c r="H4">
-        <v>46</v>
+        <v>49.2</v>
       </c>
       <c r="I4">
-        <v>44.7</v>
+        <v>49.4</v>
       </c>
       <c r="J4">
-        <v>43.6</v>
+        <v>49.6</v>
       </c>
       <c r="K4">
-        <v>42.7</v>
+        <v>50</v>
       </c>
       <c r="L4">
-        <v>41.9</v>
+        <v>50.3</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -597,37 +597,37 @@
         <v>3</v>
       </c>
       <c r="B5">
+        <v>74.40000000000001</v>
+      </c>
+      <c r="C5">
         <v>74.09999999999999</v>
       </c>
-      <c r="C5">
-        <v>74.40000000000001</v>
-      </c>
       <c r="D5">
-        <v>74.40000000000001</v>
+        <v>73.40000000000001</v>
       </c>
       <c r="E5">
-        <v>74.09999999999999</v>
+        <v>72.59999999999999</v>
       </c>
       <c r="F5">
-        <v>73.59999999999999</v>
+        <v>71.59999999999999</v>
       </c>
       <c r="G5">
-        <v>72.90000000000001</v>
+        <v>70.5</v>
       </c>
       <c r="H5">
-        <v>72.2</v>
+        <v>69.3</v>
       </c>
       <c r="I5">
-        <v>71.3</v>
+        <v>68</v>
       </c>
       <c r="J5">
-        <v>70.40000000000001</v>
+        <v>66.7</v>
       </c>
       <c r="K5">
-        <v>69.5</v>
+        <v>65.3</v>
       </c>
       <c r="L5">
-        <v>68.5</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -635,37 +635,37 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>69.59999999999999</v>
+        <v>63.1</v>
       </c>
       <c r="C6">
-        <v>64.90000000000001</v>
+        <v>61.1</v>
       </c>
       <c r="D6">
-        <v>60.1</v>
+        <v>60.4</v>
       </c>
       <c r="E6">
-        <v>55.4</v>
+        <v>61</v>
       </c>
       <c r="F6">
-        <v>51.1</v>
+        <v>62.8</v>
       </c>
       <c r="G6">
-        <v>47.1</v>
+        <v>65.90000000000001</v>
       </c>
       <c r="H6">
-        <v>43.6</v>
+        <v>70</v>
       </c>
       <c r="I6">
-        <v>40.7</v>
+        <v>74.7</v>
       </c>
       <c r="J6">
-        <v>38.3</v>
+        <v>79.8</v>
       </c>
       <c r="K6">
-        <v>36.5</v>
+        <v>84.8</v>
       </c>
       <c r="L6">
-        <v>35.4</v>
+        <v>89.40000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -673,37 +673,37 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>76.5</v>
+        <v>69.90000000000001</v>
       </c>
       <c r="C7">
-        <v>72.59999999999999</v>
+        <v>67.40000000000001</v>
       </c>
       <c r="D7">
-        <v>68.8</v>
+        <v>65.59999999999999</v>
       </c>
       <c r="E7">
-        <v>65.3</v>
+        <v>64.59999999999999</v>
       </c>
       <c r="F7">
-        <v>62.2</v>
+        <v>64.09999999999999</v>
       </c>
       <c r="G7">
-        <v>59.4</v>
+        <v>64.09999999999999</v>
       </c>
       <c r="H7">
-        <v>56.8</v>
+        <v>64.2</v>
       </c>
       <c r="I7">
-        <v>54.4</v>
+        <v>64.40000000000001</v>
       </c>
       <c r="J7">
-        <v>52.1</v>
+        <v>64.5</v>
       </c>
       <c r="K7">
-        <v>49.7</v>
+        <v>64.40000000000001</v>
       </c>
       <c r="L7">
-        <v>47.2</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -711,37 +711,37 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>80.7</v>
+        <v>80.8</v>
       </c>
       <c r="C8">
-        <v>80.90000000000001</v>
+        <v>80.3</v>
       </c>
       <c r="D8">
-        <v>80.8</v>
+        <v>79.8</v>
       </c>
       <c r="E8">
-        <v>80.5</v>
+        <v>79.2</v>
       </c>
       <c r="F8">
-        <v>80.09999999999999</v>
+        <v>78.7</v>
       </c>
       <c r="G8">
-        <v>79.7</v>
+        <v>78.2</v>
       </c>
       <c r="H8">
-        <v>79.5</v>
+        <v>77.8</v>
       </c>
       <c r="I8">
-        <v>79.40000000000001</v>
+        <v>77.3</v>
       </c>
       <c r="J8">
-        <v>79.40000000000001</v>
+        <v>76.7</v>
       </c>
       <c r="K8">
-        <v>79.3</v>
+        <v>75.90000000000001</v>
       </c>
       <c r="L8">
-        <v>79.2</v>
+        <v>74.90000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -749,37 +749,37 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>78.7</v>
+        <v>77.09999999999999</v>
       </c>
       <c r="C9">
-        <v>78.09999999999999</v>
+        <v>76</v>
       </c>
       <c r="D9">
-        <v>77.40000000000001</v>
+        <v>75</v>
       </c>
       <c r="E9">
-        <v>76.7</v>
+        <v>74</v>
       </c>
       <c r="F9">
-        <v>76.09999999999999</v>
+        <v>73</v>
       </c>
       <c r="G9">
-        <v>75.7</v>
+        <v>72</v>
       </c>
       <c r="H9">
-        <v>75.5</v>
+        <v>70.8</v>
       </c>
       <c r="I9">
-        <v>75.2</v>
+        <v>69.40000000000001</v>
       </c>
       <c r="J9">
-        <v>74.90000000000001</v>
+        <v>67.7</v>
       </c>
       <c r="K9">
-        <v>74.40000000000001</v>
+        <v>65.7</v>
       </c>
       <c r="L9">
-        <v>73.59999999999999</v>
+        <v>63.6</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -787,37 +787,37 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>79.8</v>
+        <v>79.90000000000001</v>
       </c>
       <c r="C10">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D10">
-        <v>79.40000000000001</v>
+        <v>77.59999999999999</v>
       </c>
       <c r="E10">
-        <v>78</v>
+        <v>75.8</v>
       </c>
       <c r="F10">
-        <v>75.90000000000001</v>
+        <v>73.7</v>
       </c>
       <c r="G10">
-        <v>73.2</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="H10">
-        <v>70.09999999999999</v>
+        <v>69.09999999999999</v>
       </c>
       <c r="I10">
         <v>66.7</v>
       </c>
       <c r="J10">
-        <v>63.2</v>
+        <v>64.5</v>
       </c>
       <c r="K10">
-        <v>59.6</v>
+        <v>62.3</v>
       </c>
       <c r="L10">
-        <v>56.1</v>
+        <v>60.5</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -825,37 +825,37 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>85.2</v>
+        <v>85.3</v>
       </c>
       <c r="C11">
-        <v>85.3</v>
+        <v>85</v>
       </c>
       <c r="D11">
-        <v>85.3</v>
+        <v>84.7</v>
       </c>
       <c r="E11">
-        <v>85.09999999999999</v>
+        <v>84.2</v>
       </c>
       <c r="F11">
-        <v>84.90000000000001</v>
+        <v>83.7</v>
       </c>
       <c r="G11">
-        <v>84.7</v>
+        <v>82.90000000000001</v>
       </c>
       <c r="H11">
-        <v>84.3</v>
+        <v>81.90000000000001</v>
       </c>
       <c r="I11">
-        <v>83.8</v>
+        <v>80.7</v>
       </c>
       <c r="J11">
-        <v>83.2</v>
+        <v>79.09999999999999</v>
       </c>
       <c r="K11">
-        <v>82.2</v>
+        <v>77.2</v>
       </c>
       <c r="L11">
-        <v>81</v>
+        <v>75.09999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -863,37 +863,37 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>70.8</v>
+        <v>72.3</v>
       </c>
       <c r="C12">
-        <v>71.8</v>
+        <v>72.40000000000001</v>
       </c>
       <c r="D12">
-        <v>72.3</v>
+        <v>72.09999999999999</v>
       </c>
       <c r="E12">
-        <v>72.40000000000001</v>
+        <v>71.59999999999999</v>
       </c>
       <c r="F12">
-        <v>72.2</v>
+        <v>70.90000000000001</v>
       </c>
       <c r="G12">
-        <v>71.8</v>
+        <v>70</v>
       </c>
       <c r="H12">
-        <v>71.2</v>
+        <v>69</v>
       </c>
       <c r="I12">
-        <v>70.5</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="J12">
-        <v>69.8</v>
+        <v>66.7</v>
       </c>
       <c r="K12">
-        <v>68.90000000000001</v>
+        <v>65.40000000000001</v>
       </c>
       <c r="L12">
-        <v>67.90000000000001</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -901,37 +901,37 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>68.90000000000001</v>
+        <v>69.09999999999999</v>
       </c>
       <c r="C13">
-        <v>68.90000000000001</v>
+        <v>68.8</v>
       </c>
       <c r="D13">
-        <v>68.5</v>
+        <v>68.3</v>
       </c>
       <c r="E13">
-        <v>67.7</v>
+        <v>67.59999999999999</v>
       </c>
       <c r="F13">
-        <v>66.5</v>
+        <v>66.90000000000001</v>
       </c>
       <c r="G13">
-        <v>65</v>
+        <v>66.09999999999999</v>
       </c>
       <c r="H13">
-        <v>63.3</v>
+        <v>65.2</v>
       </c>
       <c r="I13">
-        <v>61.4</v>
+        <v>64.40000000000001</v>
       </c>
       <c r="J13">
-        <v>59.4</v>
+        <v>63.5</v>
       </c>
       <c r="K13">
-        <v>57.4</v>
+        <v>62.7</v>
       </c>
       <c r="L13">
-        <v>55.4</v>
+        <v>61.8</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -939,37 +939,37 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>85.59999999999999</v>
+        <v>77</v>
       </c>
       <c r="C14">
-        <v>81.09999999999999</v>
+        <v>73.3</v>
       </c>
       <c r="D14">
-        <v>76.90000000000001</v>
+        <v>70.3</v>
       </c>
       <c r="E14">
-        <v>73</v>
+        <v>68.2</v>
       </c>
       <c r="F14">
-        <v>69.90000000000001</v>
+        <v>67</v>
       </c>
       <c r="G14">
-        <v>67.7</v>
+        <v>66.59999999999999</v>
       </c>
       <c r="H14">
-        <v>66.3</v>
+        <v>66.8</v>
       </c>
       <c r="I14">
-        <v>65.59999999999999</v>
+        <v>67.40000000000001</v>
       </c>
       <c r="J14">
-        <v>65.59999999999999</v>
+        <v>68.2</v>
       </c>
       <c r="K14">
-        <v>66</v>
+        <v>68.90000000000001</v>
       </c>
       <c r="L14">
-        <v>66.59999999999999</v>
+        <v>69.5</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -977,37 +977,37 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>79.40000000000001</v>
+        <v>77.8</v>
       </c>
       <c r="C15">
-        <v>78.7</v>
+        <v>77.3</v>
       </c>
       <c r="D15">
-        <v>78.09999999999999</v>
+        <v>76.90000000000001</v>
       </c>
       <c r="E15">
-        <v>77.8</v>
+        <v>76.7</v>
       </c>
       <c r="F15">
-        <v>77.8</v>
+        <v>76.7</v>
       </c>
       <c r="G15">
-        <v>78</v>
+        <v>76.59999999999999</v>
       </c>
       <c r="H15">
-        <v>78.5</v>
+        <v>76.40000000000001</v>
       </c>
       <c r="I15">
-        <v>79.09999999999999</v>
+        <v>76</v>
       </c>
       <c r="J15">
-        <v>79.5</v>
+        <v>75.09999999999999</v>
       </c>
       <c r="K15">
-        <v>79.7</v>
+        <v>73.8</v>
       </c>
       <c r="L15">
-        <v>79.5</v>
+        <v>72.09999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1015,37 +1015,37 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>63.6</v>
+        <v>63</v>
       </c>
       <c r="C16">
-        <v>63.1</v>
+        <v>62.4</v>
       </c>
       <c r="D16">
-        <v>62.3</v>
+        <v>61.7</v>
       </c>
       <c r="E16">
         <v>61.1</v>
       </c>
       <c r="F16">
+        <v>60.5</v>
+      </c>
+      <c r="G16">
+        <v>60</v>
+      </c>
+      <c r="H16">
+        <v>59.7</v>
+      </c>
+      <c r="I16">
+        <v>59.5</v>
+      </c>
+      <c r="J16">
+        <v>59.5</v>
+      </c>
+      <c r="K16">
         <v>59.6</v>
       </c>
-      <c r="G16">
-        <v>57.9</v>
-      </c>
-      <c r="H16">
-        <v>56.1</v>
-      </c>
-      <c r="I16">
-        <v>54.3</v>
-      </c>
-      <c r="J16">
-        <v>52.5</v>
-      </c>
-      <c r="K16">
-        <v>50.9</v>
-      </c>
       <c r="L16">
-        <v>49.4</v>
+        <v>59.8</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1053,37 +1053,37 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>69.7</v>
+        <v>69.40000000000001</v>
       </c>
       <c r="C17">
-        <v>69.40000000000001</v>
+        <v>69</v>
       </c>
       <c r="D17">
         <v>68.7</v>
       </c>
       <c r="E17">
-        <v>67.8</v>
+        <v>68.5</v>
       </c>
       <c r="F17">
-        <v>66.59999999999999</v>
+        <v>68.5</v>
       </c>
       <c r="G17">
-        <v>65.40000000000001</v>
+        <v>68.59999999999999</v>
       </c>
       <c r="H17">
-        <v>64.09999999999999</v>
+        <v>68.8</v>
       </c>
       <c r="I17">
-        <v>62.8</v>
+        <v>69.2</v>
       </c>
       <c r="J17">
-        <v>61.6</v>
+        <v>69.59999999999999</v>
       </c>
       <c r="K17">
-        <v>60.4</v>
+        <v>70</v>
       </c>
       <c r="L17">
-        <v>59.3</v>
+        <v>70.2</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1091,37 +1091,37 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>74.40000000000001</v>
+        <v>74.3</v>
       </c>
       <c r="C18">
-        <v>74.59999999999999</v>
+        <v>74</v>
       </c>
       <c r="D18">
-        <v>74.7</v>
+        <v>73.5</v>
       </c>
       <c r="E18">
-        <v>74.7</v>
+        <v>73</v>
       </c>
       <c r="F18">
-        <v>74.7</v>
+        <v>72.3</v>
       </c>
       <c r="G18">
-        <v>74.7</v>
+        <v>71.5</v>
       </c>
       <c r="H18">
-        <v>74.7</v>
+        <v>70.5</v>
       </c>
       <c r="I18">
-        <v>74.7</v>
+        <v>69.3</v>
       </c>
       <c r="J18">
-        <v>74.5</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="K18">
-        <v>74.09999999999999</v>
+        <v>66.3</v>
       </c>
       <c r="L18">
-        <v>73.5</v>
+        <v>64.59999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1129,37 +1129,37 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>73.3</v>
+        <v>64.3</v>
       </c>
       <c r="C19">
-        <v>68.3</v>
+        <v>60.5</v>
       </c>
       <c r="D19">
-        <v>63.3</v>
+        <v>57.5</v>
       </c>
       <c r="E19">
-        <v>58.5</v>
+        <v>55.5</v>
       </c>
       <c r="F19">
-        <v>54.2</v>
+        <v>54.5</v>
       </c>
       <c r="G19">
-        <v>50.6</v>
+        <v>54.4</v>
       </c>
       <c r="H19">
-        <v>47.5</v>
+        <v>55.1</v>
       </c>
       <c r="I19">
-        <v>45.2</v>
+        <v>56.3</v>
       </c>
       <c r="J19">
-        <v>43.4</v>
+        <v>57.9</v>
       </c>
       <c r="K19">
-        <v>42.1</v>
+        <v>59.6</v>
       </c>
       <c r="L19">
-        <v>41.3</v>
+        <v>61.2</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1167,37 +1167,37 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>79.5</v>
+        <v>72.40000000000001</v>
       </c>
       <c r="C20">
-        <v>75.59999999999999</v>
+        <v>70</v>
       </c>
       <c r="D20">
-        <v>72.3</v>
+        <v>68.59999999999999</v>
       </c>
       <c r="E20">
-        <v>69.8</v>
+        <v>68.3</v>
       </c>
       <c r="F20">
-        <v>68.2</v>
+        <v>68.7</v>
       </c>
       <c r="G20">
-        <v>67.59999999999999</v>
+        <v>69.7</v>
       </c>
       <c r="H20">
-        <v>67.8</v>
+        <v>71.09999999999999</v>
       </c>
       <c r="I20">
-        <v>68.59999999999999</v>
+        <v>72.40000000000001</v>
       </c>
       <c r="J20">
-        <v>69.59999999999999</v>
+        <v>73.40000000000001</v>
       </c>
       <c r="K20">
-        <v>70.59999999999999</v>
+        <v>73.90000000000001</v>
       </c>
       <c r="L20">
-        <v>71.3</v>
+        <v>73.8</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1205,37 +1205,37 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>69.3</v>
+        <v>65.2</v>
       </c>
       <c r="C21">
-        <v>67.2</v>
+        <v>63.1</v>
       </c>
       <c r="D21">
-        <v>64.8</v>
+        <v>61.1</v>
       </c>
       <c r="E21">
-        <v>62.2</v>
+        <v>59.5</v>
       </c>
       <c r="F21">
-        <v>59.7</v>
+        <v>58.3</v>
       </c>
       <c r="G21">
+        <v>57.5</v>
+      </c>
+      <c r="H21">
+        <v>57.1</v>
+      </c>
+      <c r="I21">
+        <v>57</v>
+      </c>
+      <c r="J21">
+        <v>57.1</v>
+      </c>
+      <c r="K21">
         <v>57.4</v>
       </c>
-      <c r="H21">
-        <v>55.3</v>
-      </c>
-      <c r="I21">
-        <v>53.6</v>
-      </c>
-      <c r="J21">
-        <v>52.1</v>
-      </c>
-      <c r="K21">
-        <v>51</v>
-      </c>
       <c r="L21">
-        <v>50.1</v>
+        <v>57.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
forecast update last observation 21-1-25
</commit_message>
<xml_diff>
--- a/passage_clusters/VIIRS/CLUSTER_1/VCI3M_Forecast_Overview_CLUSTER_1.xlsx
+++ b/passage_clusters/VIIRS/CLUSTER_1/VCI3M_Forecast_Overview_CLUSTER_1.xlsx
@@ -445,37 +445,37 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="B1" s="1">
-        <v>45664</v>
+        <v>45678</v>
       </c>
       <c r="C1" s="1">
-        <v>45671</v>
+        <v>45685</v>
       </c>
       <c r="D1" s="1">
-        <v>45678</v>
+        <v>45692</v>
       </c>
       <c r="E1" s="1">
-        <v>45685</v>
+        <v>45699</v>
       </c>
       <c r="F1" s="1">
-        <v>45692</v>
+        <v>45706</v>
       </c>
       <c r="G1" s="1">
-        <v>45699</v>
+        <v>45713</v>
       </c>
       <c r="H1" s="1">
-        <v>45706</v>
+        <v>45720</v>
       </c>
       <c r="I1" s="1">
-        <v>45713</v>
+        <v>45727</v>
       </c>
       <c r="J1" s="1">
-        <v>45720</v>
+        <v>45734</v>
       </c>
       <c r="K1" s="1">
-        <v>45727</v>
+        <v>45741</v>
       </c>
       <c r="L1" s="1">
-        <v>45734</v>
+        <v>45748</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -483,37 +483,37 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>64.5</v>
+        <v>61.9</v>
       </c>
       <c r="C2">
-        <v>63</v>
+        <v>60.7</v>
       </c>
       <c r="D2">
-        <v>61.2</v>
+        <v>59.5</v>
       </c>
       <c r="E2">
-        <v>59.3</v>
+        <v>58.5</v>
       </c>
       <c r="F2">
-        <v>57.1</v>
+        <v>57.5</v>
       </c>
       <c r="G2">
-        <v>54.7</v>
+        <v>56.8</v>
       </c>
       <c r="H2">
-        <v>52.2</v>
+        <v>56.3</v>
       </c>
       <c r="I2">
-        <v>49.7</v>
+        <v>56.1</v>
       </c>
       <c r="J2">
-        <v>47.2</v>
+        <v>56.2</v>
       </c>
       <c r="K2">
-        <v>45</v>
+        <v>56.6</v>
       </c>
       <c r="L2">
-        <v>43.2</v>
+        <v>57.2</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -521,37 +521,37 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>59.9</v>
+        <v>62.4</v>
       </c>
       <c r="C3">
-        <v>61</v>
+        <v>63.8</v>
       </c>
       <c r="D3">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E3">
-        <v>62.8</v>
+        <v>66.2</v>
       </c>
       <c r="F3">
-        <v>63.4</v>
+        <v>67.2</v>
       </c>
       <c r="G3">
-        <v>63.7</v>
+        <v>68</v>
       </c>
       <c r="H3">
-        <v>63.7</v>
+        <v>68.5</v>
       </c>
       <c r="I3">
-        <v>63.3</v>
+        <v>68.8</v>
       </c>
       <c r="J3">
-        <v>62.5</v>
+        <v>68.8</v>
       </c>
       <c r="K3">
-        <v>61.5</v>
+        <v>68.5</v>
       </c>
       <c r="L3">
-        <v>60.1</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -559,37 +559,37 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>46.3</v>
+        <v>43.4</v>
       </c>
       <c r="C4">
-        <v>44.7</v>
+        <v>42</v>
       </c>
       <c r="D4">
-        <v>42.9</v>
+        <v>40.6</v>
       </c>
       <c r="E4">
-        <v>40.9</v>
+        <v>39.4</v>
       </c>
       <c r="F4">
-        <v>38.7</v>
+        <v>38.3</v>
       </c>
       <c r="G4">
-        <v>36.3</v>
+        <v>37.5</v>
       </c>
       <c r="H4">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="I4">
-        <v>31.6</v>
+        <v>36.9</v>
       </c>
       <c r="J4">
-        <v>29.5</v>
+        <v>37.3</v>
       </c>
       <c r="K4">
-        <v>27.7</v>
+        <v>38</v>
       </c>
       <c r="L4">
-        <v>26.3</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -597,37 +597,37 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>69.40000000000001</v>
+        <v>65.90000000000001</v>
       </c>
       <c r="C5">
-        <v>67.40000000000001</v>
+        <v>64</v>
       </c>
       <c r="D5">
-        <v>65.09999999999999</v>
+        <v>62.2</v>
       </c>
       <c r="E5">
-        <v>62.6</v>
+        <v>60.6</v>
       </c>
       <c r="F5">
-        <v>59.8</v>
+        <v>59.2</v>
       </c>
       <c r="G5">
+        <v>58</v>
+      </c>
+      <c r="H5">
+        <v>57.3</v>
+      </c>
+      <c r="I5">
         <v>56.9</v>
       </c>
-      <c r="H5">
-        <v>54</v>
-      </c>
-      <c r="I5">
-        <v>51.2</v>
-      </c>
       <c r="J5">
-        <v>48.7</v>
+        <v>56.9</v>
       </c>
       <c r="K5">
-        <v>46.5</v>
+        <v>57.3</v>
       </c>
       <c r="L5">
-        <v>44.7</v>
+        <v>57.9</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -635,37 +635,37 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>59.9</v>
+        <v>62.5</v>
       </c>
       <c r="C6">
-        <v>60.7</v>
+        <v>64.09999999999999</v>
       </c>
       <c r="D6">
-        <v>61.4</v>
+        <v>65.7</v>
       </c>
       <c r="E6">
-        <v>61.9</v>
+        <v>67</v>
       </c>
       <c r="F6">
-        <v>61.9</v>
+        <v>68.09999999999999</v>
       </c>
       <c r="G6">
-        <v>61.3</v>
+        <v>68.8</v>
       </c>
       <c r="H6">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="I6">
-        <v>58</v>
+        <v>68.8</v>
       </c>
       <c r="J6">
-        <v>55.4</v>
+        <v>68.3</v>
       </c>
       <c r="K6">
-        <v>52.2</v>
+        <v>67.40000000000001</v>
       </c>
       <c r="L6">
-        <v>48.7</v>
+        <v>66.3</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -673,37 +673,37 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>62.7</v>
+        <v>61</v>
       </c>
       <c r="C7">
-        <v>61.5</v>
+        <v>60</v>
       </c>
       <c r="D7">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E7">
-        <v>57.9</v>
+        <v>58</v>
       </c>
       <c r="F7">
-        <v>55.2</v>
+        <v>57.2</v>
       </c>
       <c r="G7">
-        <v>52.1</v>
+        <v>56.5</v>
       </c>
       <c r="H7">
-        <v>48.6</v>
+        <v>56.3</v>
       </c>
       <c r="I7">
-        <v>45</v>
+        <v>56.5</v>
       </c>
       <c r="J7">
-        <v>41.5</v>
+        <v>57.1</v>
       </c>
       <c r="K7">
-        <v>38.3</v>
+        <v>58.2</v>
       </c>
       <c r="L7">
-        <v>35.6</v>
+        <v>59.5</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -711,37 +711,37 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>74.3</v>
+        <v>70.3</v>
       </c>
       <c r="C8">
-        <v>72</v>
+        <v>68.3</v>
       </c>
       <c r="D8">
-        <v>69.5</v>
+        <v>66.3</v>
       </c>
       <c r="E8">
-        <v>66.59999999999999</v>
+        <v>64.40000000000001</v>
       </c>
       <c r="F8">
-        <v>63.4</v>
+        <v>62.7</v>
       </c>
       <c r="G8">
-        <v>60.1</v>
+        <v>61.3</v>
       </c>
       <c r="H8">
-        <v>56.7</v>
+        <v>60.2</v>
       </c>
       <c r="I8">
-        <v>53.3</v>
+        <v>59.6</v>
       </c>
       <c r="J8">
-        <v>50.1</v>
+        <v>59.4</v>
       </c>
       <c r="K8">
-        <v>47.3</v>
+        <v>59.6</v>
       </c>
       <c r="L8">
-        <v>45</v>
+        <v>60.2</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -749,37 +749,37 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>68.09999999999999</v>
+        <v>63</v>
       </c>
       <c r="C9">
-        <v>65.3</v>
+        <v>60.4</v>
       </c>
       <c r="D9">
-        <v>62.2</v>
+        <v>57.9</v>
       </c>
       <c r="E9">
-        <v>58.8</v>
+        <v>55.5</v>
       </c>
       <c r="F9">
-        <v>55.2</v>
+        <v>53.6</v>
       </c>
       <c r="G9">
+        <v>52.2</v>
+      </c>
+      <c r="H9">
         <v>51.5</v>
       </c>
-      <c r="H9">
-        <v>48</v>
-      </c>
       <c r="I9">
-        <v>44.8</v>
+        <v>51.5</v>
       </c>
       <c r="J9">
-        <v>42.2</v>
+        <v>52.2</v>
       </c>
       <c r="K9">
-        <v>40.3</v>
+        <v>53.6</v>
       </c>
       <c r="L9">
-        <v>39.1</v>
+        <v>55.4</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -787,37 +787,37 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>70.40000000000001</v>
+        <v>63.7</v>
       </c>
       <c r="C10">
-        <v>67</v>
+        <v>60.2</v>
       </c>
       <c r="D10">
-        <v>63.1</v>
+        <v>56.8</v>
       </c>
       <c r="E10">
-        <v>59.1</v>
+        <v>53.7</v>
       </c>
       <c r="F10">
-        <v>54.8</v>
+        <v>50.9</v>
       </c>
       <c r="G10">
-        <v>50.6</v>
+        <v>48.7</v>
       </c>
       <c r="H10">
-        <v>46.6</v>
+        <v>47</v>
       </c>
       <c r="I10">
-        <v>42.9</v>
+        <v>46</v>
       </c>
       <c r="J10">
-        <v>39.6</v>
+        <v>45.7</v>
       </c>
       <c r="K10">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="L10">
-        <v>35.1</v>
+        <v>46.8</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -825,37 +825,37 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>79.5</v>
+        <v>74.90000000000001</v>
       </c>
       <c r="C11">
-        <v>77.09999999999999</v>
+        <v>72.2</v>
       </c>
       <c r="D11">
-        <v>74.2</v>
+        <v>69.40000000000001</v>
       </c>
       <c r="E11">
-        <v>71</v>
+        <v>66.7</v>
       </c>
       <c r="F11">
-        <v>67.40000000000001</v>
+        <v>64.2</v>
       </c>
       <c r="G11">
-        <v>63.6</v>
+        <v>62</v>
       </c>
       <c r="H11">
-        <v>59.8</v>
+        <v>60.3</v>
       </c>
       <c r="I11">
-        <v>56.2</v>
+        <v>59.1</v>
       </c>
       <c r="J11">
-        <v>53</v>
+        <v>58.5</v>
       </c>
       <c r="K11">
-        <v>50.2</v>
+        <v>58.5</v>
       </c>
       <c r="L11">
-        <v>48.1</v>
+        <v>58.9</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -863,37 +863,37 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>69.40000000000001</v>
+        <v>66.7</v>
       </c>
       <c r="C12">
-        <v>68</v>
+        <v>65.2</v>
       </c>
       <c r="D12">
-        <v>66.5</v>
+        <v>63.7</v>
       </c>
       <c r="E12">
-        <v>64.90000000000001</v>
+        <v>62.1</v>
       </c>
       <c r="F12">
-        <v>63.1</v>
+        <v>60.5</v>
       </c>
       <c r="G12">
-        <v>61.3</v>
+        <v>58.9</v>
       </c>
       <c r="H12">
-        <v>59.4</v>
+        <v>57.5</v>
       </c>
       <c r="I12">
-        <v>57.6</v>
+        <v>56.3</v>
       </c>
       <c r="J12">
-        <v>55.8</v>
+        <v>55.2</v>
       </c>
       <c r="K12">
-        <v>54.3</v>
+        <v>54.4</v>
       </c>
       <c r="L12">
-        <v>52.9</v>
+        <v>53.8</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -901,37 +901,37 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>65.8</v>
+        <v>63.3</v>
       </c>
       <c r="C13">
-        <v>64.59999999999999</v>
+        <v>62</v>
       </c>
       <c r="D13">
-        <v>63.1</v>
+        <v>60.5</v>
       </c>
       <c r="E13">
-        <v>61.5</v>
+        <v>59.1</v>
       </c>
       <c r="F13">
-        <v>59.7</v>
+        <v>57.6</v>
       </c>
       <c r="G13">
-        <v>57.8</v>
+        <v>56.3</v>
       </c>
       <c r="H13">
-        <v>55.8</v>
+        <v>55</v>
       </c>
       <c r="I13">
-        <v>53.8</v>
+        <v>53.9</v>
       </c>
       <c r="J13">
-        <v>51.8</v>
+        <v>53</v>
       </c>
       <c r="K13">
-        <v>49.9</v>
+        <v>52.2</v>
       </c>
       <c r="L13">
-        <v>48.2</v>
+        <v>51.6</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -939,37 +939,37 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>60.9</v>
+        <v>58.3</v>
       </c>
       <c r="C14">
-        <v>58.9</v>
+        <v>58.2</v>
       </c>
       <c r="D14">
-        <v>56.9</v>
+        <v>58.6</v>
       </c>
       <c r="E14">
-        <v>55.1</v>
+        <v>59.7</v>
       </c>
       <c r="F14">
-        <v>53.2</v>
+        <v>61.4</v>
       </c>
       <c r="G14">
-        <v>51.2</v>
+        <v>63.7</v>
       </c>
       <c r="H14">
-        <v>49.2</v>
+        <v>66.5</v>
       </c>
       <c r="I14">
-        <v>47.2</v>
+        <v>69.8</v>
       </c>
       <c r="J14">
-        <v>45.4</v>
+        <v>73.40000000000001</v>
       </c>
       <c r="K14">
-        <v>43.8</v>
+        <v>77</v>
       </c>
       <c r="L14">
-        <v>42.5</v>
+        <v>80.59999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -977,37 +977,37 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>70.3</v>
+        <v>64.8</v>
       </c>
       <c r="C15">
-        <v>67.3</v>
+        <v>61.7</v>
       </c>
       <c r="D15">
-        <v>63.7</v>
+        <v>58.6</v>
       </c>
       <c r="E15">
-        <v>59.5</v>
+        <v>55.6</v>
       </c>
       <c r="F15">
-        <v>54.9</v>
+        <v>52.9</v>
       </c>
       <c r="G15">
-        <v>49.9</v>
+        <v>50.8</v>
       </c>
       <c r="H15">
-        <v>44.9</v>
+        <v>49.4</v>
       </c>
       <c r="I15">
-        <v>40.2</v>
+        <v>48.8</v>
       </c>
       <c r="J15">
-        <v>35.9</v>
+        <v>49</v>
       </c>
       <c r="K15">
-        <v>32.4</v>
+        <v>50.1</v>
       </c>
       <c r="L15">
-        <v>29.9</v>
+        <v>51.8</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1015,37 +1015,37 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>58.4</v>
+        <v>56</v>
       </c>
       <c r="C16">
-        <v>57.2</v>
+        <v>54.9</v>
       </c>
       <c r="D16">
-        <v>55.9</v>
+        <v>53.9</v>
       </c>
       <c r="E16">
-        <v>54.6</v>
+        <v>52.9</v>
       </c>
       <c r="F16">
-        <v>53.3</v>
+        <v>52.1</v>
       </c>
       <c r="G16">
-        <v>52</v>
+        <v>51.3</v>
       </c>
       <c r="H16">
         <v>50.7</v>
       </c>
       <c r="I16">
-        <v>49.5</v>
+        <v>50.1</v>
       </c>
       <c r="J16">
-        <v>48.3</v>
+        <v>49.7</v>
       </c>
       <c r="K16">
-        <v>47.2</v>
+        <v>49.4</v>
       </c>
       <c r="L16">
-        <v>46.2</v>
+        <v>49.2</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1053,37 +1053,37 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>65.7</v>
+        <v>63.3</v>
       </c>
       <c r="C17">
-        <v>64.5</v>
+        <v>62.1</v>
       </c>
       <c r="D17">
-        <v>63.1</v>
+        <v>60.8</v>
       </c>
       <c r="E17">
-        <v>61.5</v>
+        <v>59.4</v>
       </c>
       <c r="F17">
-        <v>59.6</v>
+        <v>58.1</v>
       </c>
       <c r="G17">
-        <v>57.6</v>
+        <v>56.7</v>
       </c>
       <c r="H17">
-        <v>55.5</v>
+        <v>55.4</v>
       </c>
       <c r="I17">
-        <v>53.2</v>
+        <v>54.3</v>
       </c>
       <c r="J17">
-        <v>51</v>
+        <v>53.4</v>
       </c>
       <c r="K17">
-        <v>48.8</v>
+        <v>52.6</v>
       </c>
       <c r="L17">
-        <v>46.8</v>
+        <v>52.1</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1091,37 +1091,37 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>67.90000000000001</v>
+        <v>63.6</v>
       </c>
       <c r="C18">
-        <v>65.5</v>
+        <v>61.3</v>
       </c>
       <c r="D18">
-        <v>62.9</v>
+        <v>59.2</v>
       </c>
       <c r="E18">
-        <v>60.1</v>
+        <v>57.3</v>
       </c>
       <c r="F18">
-        <v>57.2</v>
+        <v>55.8</v>
       </c>
       <c r="G18">
+        <v>54.7</v>
+      </c>
+      <c r="H18">
+        <v>54.2</v>
+      </c>
+      <c r="I18">
         <v>54.3</v>
       </c>
-      <c r="H18">
-        <v>51.5</v>
-      </c>
-      <c r="I18">
-        <v>49.1</v>
-      </c>
       <c r="J18">
-        <v>47.1</v>
+        <v>54.9</v>
       </c>
       <c r="K18">
-        <v>45.7</v>
+        <v>56.1</v>
       </c>
       <c r="L18">
-        <v>45</v>
+        <v>57.6</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1129,37 +1129,37 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>54.4</v>
+        <v>55.2</v>
       </c>
       <c r="C19">
-        <v>54.3</v>
+        <v>56.2</v>
       </c>
       <c r="D19">
-        <v>54.4</v>
+        <v>57.3</v>
       </c>
       <c r="E19">
-        <v>54.5</v>
+        <v>58.4</v>
       </c>
       <c r="F19">
-        <v>54.3</v>
+        <v>59.4</v>
       </c>
       <c r="G19">
-        <v>53.7</v>
+        <v>60.3</v>
       </c>
       <c r="H19">
-        <v>52.6</v>
+        <v>61</v>
       </c>
       <c r="I19">
-        <v>51</v>
+        <v>61.5</v>
       </c>
       <c r="J19">
-        <v>49</v>
+        <v>61.8</v>
       </c>
       <c r="K19">
-        <v>46.7</v>
+        <v>62</v>
       </c>
       <c r="L19">
-        <v>44.2</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1167,37 +1167,37 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>64.90000000000001</v>
+        <v>64.40000000000001</v>
       </c>
       <c r="C20">
+        <v>64.3</v>
+      </c>
+      <c r="D20">
+        <v>64.09999999999999</v>
+      </c>
+      <c r="E20">
+        <v>63.9</v>
+      </c>
+      <c r="F20">
+        <v>63.8</v>
+      </c>
+      <c r="G20">
+        <v>63.8</v>
+      </c>
+      <c r="H20">
         <v>64.2</v>
       </c>
-      <c r="D20">
-        <v>63.2</v>
-      </c>
-      <c r="E20">
-        <v>61.7</v>
-      </c>
-      <c r="F20">
-        <v>59.7</v>
-      </c>
-      <c r="G20">
-        <v>57.1</v>
-      </c>
-      <c r="H20">
-        <v>54.3</v>
-      </c>
       <c r="I20">
-        <v>51.2</v>
+        <v>65</v>
       </c>
       <c r="J20">
-        <v>48.2</v>
+        <v>66.09999999999999</v>
       </c>
       <c r="K20">
-        <v>45.4</v>
+        <v>67.59999999999999</v>
       </c>
       <c r="L20">
-        <v>43.2</v>
+        <v>69.3</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1205,37 +1205,37 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>56.5</v>
+        <v>54</v>
       </c>
       <c r="C21">
-        <v>55.1</v>
+        <v>52.9</v>
       </c>
       <c r="D21">
-        <v>53.6</v>
+        <v>51.8</v>
       </c>
       <c r="E21">
-        <v>52</v>
+        <v>50.8</v>
       </c>
       <c r="F21">
-        <v>50.3</v>
+        <v>49.8</v>
       </c>
       <c r="G21">
-        <v>48.4</v>
+        <v>48.8</v>
       </c>
       <c r="H21">
-        <v>46.4</v>
+        <v>48</v>
       </c>
       <c r="I21">
-        <v>44.3</v>
+        <v>47.3</v>
       </c>
       <c r="J21">
-        <v>42.1</v>
+        <v>46.8</v>
       </c>
       <c r="K21">
-        <v>40.1</v>
+        <v>46.6</v>
       </c>
       <c r="L21">
-        <v>38.4</v>
+        <v>46.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Beginning of Feb update
</commit_message>
<xml_diff>
--- a/passage_clusters/VIIRS/CLUSTER_1/VCI3M_Forecast_Overview_CLUSTER_1.xlsx
+++ b/passage_clusters/VIIRS/CLUSTER_1/VCI3M_Forecast_Overview_CLUSTER_1.xlsx
@@ -445,37 +445,37 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="B1" s="1">
-        <v>45678</v>
+        <v>45685</v>
       </c>
       <c r="C1" s="1">
-        <v>45685</v>
+        <v>45692</v>
       </c>
       <c r="D1" s="1">
-        <v>45692</v>
+        <v>45699</v>
       </c>
       <c r="E1" s="1">
-        <v>45699</v>
+        <v>45706</v>
       </c>
       <c r="F1" s="1">
-        <v>45706</v>
+        <v>45713</v>
       </c>
       <c r="G1" s="1">
-        <v>45713</v>
+        <v>45720</v>
       </c>
       <c r="H1" s="1">
-        <v>45720</v>
+        <v>45727</v>
       </c>
       <c r="I1" s="1">
-        <v>45727</v>
+        <v>45734</v>
       </c>
       <c r="J1" s="1">
-        <v>45734</v>
+        <v>45741</v>
       </c>
       <c r="K1" s="1">
-        <v>45741</v>
+        <v>45748</v>
       </c>
       <c r="L1" s="1">
-        <v>45748</v>
+        <v>45755</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -483,37 +483,37 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>61.9</v>
+        <v>61.1</v>
       </c>
       <c r="C2">
-        <v>60.7</v>
+        <v>60.4</v>
       </c>
       <c r="D2">
-        <v>59.5</v>
+        <v>60</v>
       </c>
       <c r="E2">
-        <v>58.5</v>
+        <v>59.9</v>
       </c>
       <c r="F2">
-        <v>57.5</v>
+        <v>60.3</v>
       </c>
       <c r="G2">
-        <v>56.8</v>
+        <v>61</v>
       </c>
       <c r="H2">
-        <v>56.3</v>
+        <v>62.3</v>
       </c>
       <c r="I2">
-        <v>56.1</v>
+        <v>63.8</v>
       </c>
       <c r="J2">
-        <v>56.2</v>
+        <v>65.7</v>
       </c>
       <c r="K2">
-        <v>56.6</v>
+        <v>67.7</v>
       </c>
       <c r="L2">
-        <v>57.2</v>
+        <v>69.7</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -521,37 +521,37 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>62.4</v>
+        <v>64.09999999999999</v>
       </c>
       <c r="C3">
-        <v>63.8</v>
+        <v>65.90000000000001</v>
       </c>
       <c r="D3">
-        <v>65</v>
+        <v>67.7</v>
       </c>
       <c r="E3">
-        <v>66.2</v>
+        <v>69.59999999999999</v>
       </c>
       <c r="F3">
-        <v>67.2</v>
+        <v>71.5</v>
       </c>
       <c r="G3">
-        <v>68</v>
+        <v>73.3</v>
       </c>
       <c r="H3">
-        <v>68.5</v>
+        <v>75</v>
       </c>
       <c r="I3">
-        <v>68.8</v>
+        <v>76.40000000000001</v>
       </c>
       <c r="J3">
-        <v>68.8</v>
+        <v>77.59999999999999</v>
       </c>
       <c r="K3">
-        <v>68.5</v>
+        <v>78.5</v>
       </c>
       <c r="L3">
-        <v>68</v>
+        <v>78.90000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -559,37 +559,37 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>43.4</v>
+        <v>42.5</v>
       </c>
       <c r="C4">
-        <v>42</v>
+        <v>41.8</v>
       </c>
       <c r="D4">
-        <v>40.6</v>
+        <v>41.5</v>
       </c>
       <c r="E4">
-        <v>39.4</v>
+        <v>41.6</v>
       </c>
       <c r="F4">
-        <v>38.3</v>
+        <v>42.3</v>
       </c>
       <c r="G4">
-        <v>37.5</v>
+        <v>43.6</v>
       </c>
       <c r="H4">
-        <v>37</v>
+        <v>45.4</v>
       </c>
       <c r="I4">
-        <v>36.9</v>
+        <v>47.7</v>
       </c>
       <c r="J4">
-        <v>37.3</v>
+        <v>50.4</v>
       </c>
       <c r="K4">
-        <v>38</v>
+        <v>53.3</v>
       </c>
       <c r="L4">
-        <v>39</v>
+        <v>56.3</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -597,37 +597,37 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>65.90000000000001</v>
+        <v>64.2</v>
       </c>
       <c r="C5">
-        <v>64</v>
+        <v>62.6</v>
       </c>
       <c r="D5">
+        <v>61.2</v>
+      </c>
+      <c r="E5">
+        <v>60.2</v>
+      </c>
+      <c r="F5">
+        <v>59.5</v>
+      </c>
+      <c r="G5">
+        <v>59.2</v>
+      </c>
+      <c r="H5">
+        <v>59.4</v>
+      </c>
+      <c r="I5">
+        <v>60</v>
+      </c>
+      <c r="J5">
+        <v>61</v>
+      </c>
+      <c r="K5">
         <v>62.2</v>
       </c>
-      <c r="E5">
-        <v>60.6</v>
-      </c>
-      <c r="F5">
-        <v>59.2</v>
-      </c>
-      <c r="G5">
-        <v>58</v>
-      </c>
-      <c r="H5">
-        <v>57.3</v>
-      </c>
-      <c r="I5">
-        <v>56.9</v>
-      </c>
-      <c r="J5">
-        <v>56.9</v>
-      </c>
-      <c r="K5">
-        <v>57.3</v>
-      </c>
       <c r="L5">
-        <v>57.9</v>
+        <v>63.6</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -635,37 +635,37 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>62.5</v>
+        <v>64.59999999999999</v>
       </c>
       <c r="C6">
-        <v>64.09999999999999</v>
+        <v>66.7</v>
       </c>
       <c r="D6">
-        <v>65.7</v>
+        <v>68.90000000000001</v>
       </c>
       <c r="E6">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F6">
-        <v>68.09999999999999</v>
+        <v>73</v>
       </c>
       <c r="G6">
-        <v>68.8</v>
+        <v>74.7</v>
       </c>
       <c r="H6">
-        <v>69</v>
+        <v>76.2</v>
       </c>
       <c r="I6">
-        <v>68.8</v>
+        <v>77.3</v>
       </c>
       <c r="J6">
-        <v>68.3</v>
+        <v>78.2</v>
       </c>
       <c r="K6">
-        <v>67.40000000000001</v>
+        <v>78.7</v>
       </c>
       <c r="L6">
-        <v>66.3</v>
+        <v>78.90000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -673,37 +673,37 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>61</v>
+        <v>60.4</v>
       </c>
       <c r="C7">
-        <v>60</v>
+        <v>59.9</v>
       </c>
       <c r="D7">
-        <v>59</v>
+        <v>59.7</v>
       </c>
       <c r="E7">
-        <v>58</v>
+        <v>59.7</v>
       </c>
       <c r="F7">
-        <v>57.2</v>
+        <v>60.2</v>
       </c>
       <c r="G7">
-        <v>56.5</v>
+        <v>61.3</v>
       </c>
       <c r="H7">
-        <v>56.3</v>
+        <v>62.9</v>
       </c>
       <c r="I7">
-        <v>56.5</v>
+        <v>65.09999999999999</v>
       </c>
       <c r="J7">
-        <v>57.1</v>
+        <v>67.59999999999999</v>
       </c>
       <c r="K7">
-        <v>58.2</v>
+        <v>70.40000000000001</v>
       </c>
       <c r="L7">
-        <v>59.5</v>
+        <v>73.2</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -711,37 +711,37 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>70.3</v>
+        <v>68.59999999999999</v>
       </c>
       <c r="C8">
-        <v>68.3</v>
+        <v>67.09999999999999</v>
       </c>
       <c r="D8">
-        <v>66.3</v>
+        <v>65.8</v>
       </c>
       <c r="E8">
-        <v>64.40000000000001</v>
+        <v>65</v>
       </c>
       <c r="F8">
-        <v>62.7</v>
+        <v>64.59999999999999</v>
       </c>
       <c r="G8">
-        <v>61.3</v>
+        <v>64.7</v>
       </c>
       <c r="H8">
-        <v>60.2</v>
+        <v>65.3</v>
       </c>
       <c r="I8">
-        <v>59.6</v>
+        <v>66.40000000000001</v>
       </c>
       <c r="J8">
-        <v>59.4</v>
+        <v>68</v>
       </c>
       <c r="K8">
-        <v>59.6</v>
+        <v>69.90000000000001</v>
       </c>
       <c r="L8">
-        <v>60.2</v>
+        <v>71.90000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -749,37 +749,37 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>63</v>
+        <v>60.8</v>
       </c>
       <c r="C9">
-        <v>60.4</v>
+        <v>58.7</v>
       </c>
       <c r="D9">
-        <v>57.9</v>
+        <v>57.1</v>
       </c>
       <c r="E9">
-        <v>55.5</v>
+        <v>56.1</v>
       </c>
       <c r="F9">
-        <v>53.6</v>
+        <v>55.8</v>
       </c>
       <c r="G9">
-        <v>52.2</v>
+        <v>56.4</v>
       </c>
       <c r="H9">
-        <v>51.5</v>
+        <v>57.8</v>
       </c>
       <c r="I9">
-        <v>51.5</v>
+        <v>60.1</v>
       </c>
       <c r="J9">
-        <v>52.2</v>
+        <v>62.9</v>
       </c>
       <c r="K9">
-        <v>53.6</v>
+        <v>66.09999999999999</v>
       </c>
       <c r="L9">
-        <v>55.4</v>
+        <v>69.5</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -787,37 +787,37 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>63.7</v>
+        <v>60.7</v>
       </c>
       <c r="C10">
-        <v>60.2</v>
+        <v>57.9</v>
       </c>
       <c r="D10">
+        <v>55.5</v>
+      </c>
+      <c r="E10">
+        <v>53.8</v>
+      </c>
+      <c r="F10">
+        <v>52.9</v>
+      </c>
+      <c r="G10">
+        <v>52.7</v>
+      </c>
+      <c r="H10">
+        <v>53.4</v>
+      </c>
+      <c r="I10">
+        <v>54.8</v>
+      </c>
+      <c r="J10">
         <v>56.8</v>
       </c>
-      <c r="E10">
-        <v>53.7</v>
-      </c>
-      <c r="F10">
-        <v>50.9</v>
-      </c>
-      <c r="G10">
-        <v>48.7</v>
-      </c>
-      <c r="H10">
-        <v>47</v>
-      </c>
-      <c r="I10">
-        <v>46</v>
-      </c>
-      <c r="J10">
-        <v>45.7</v>
-      </c>
       <c r="K10">
-        <v>46</v>
+        <v>59.3</v>
       </c>
       <c r="L10">
-        <v>46.8</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -825,37 +825,37 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>74.90000000000001</v>
+        <v>72.59999999999999</v>
       </c>
       <c r="C11">
-        <v>72.2</v>
+        <v>70.40000000000001</v>
       </c>
       <c r="D11">
-        <v>69.40000000000001</v>
+        <v>68.5</v>
       </c>
       <c r="E11">
-        <v>66.7</v>
+        <v>67</v>
       </c>
       <c r="F11">
-        <v>64.2</v>
+        <v>66.09999999999999</v>
       </c>
       <c r="G11">
-        <v>62</v>
+        <v>65.90000000000001</v>
       </c>
       <c r="H11">
-        <v>60.3</v>
+        <v>66.3</v>
       </c>
       <c r="I11">
-        <v>59.1</v>
+        <v>67.40000000000001</v>
       </c>
       <c r="J11">
-        <v>58.5</v>
+        <v>69.09999999999999</v>
       </c>
       <c r="K11">
-        <v>58.5</v>
+        <v>71.09999999999999</v>
       </c>
       <c r="L11">
-        <v>58.9</v>
+        <v>73.3</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -863,37 +863,37 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>66.7</v>
+        <v>65.3</v>
       </c>
       <c r="C12">
-        <v>65.2</v>
+        <v>63.8</v>
       </c>
       <c r="D12">
-        <v>63.7</v>
+        <v>62.3</v>
       </c>
       <c r="E12">
-        <v>62.1</v>
+        <v>60.9</v>
       </c>
       <c r="F12">
-        <v>60.5</v>
+        <v>59.5</v>
       </c>
       <c r="G12">
-        <v>58.9</v>
+        <v>58.3</v>
       </c>
       <c r="H12">
-        <v>57.5</v>
+        <v>57.3</v>
       </c>
       <c r="I12">
-        <v>56.3</v>
+        <v>56.5</v>
       </c>
       <c r="J12">
-        <v>55.2</v>
+        <v>55.9</v>
       </c>
       <c r="K12">
-        <v>54.4</v>
+        <v>55.6</v>
       </c>
       <c r="L12">
-        <v>53.8</v>
+        <v>55.4</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -901,37 +901,37 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>63.3</v>
+        <v>62.3</v>
       </c>
       <c r="C13">
+        <v>61.4</v>
+      </c>
+      <c r="D13">
+        <v>60.6</v>
+      </c>
+      <c r="E13">
+        <v>60</v>
+      </c>
+      <c r="F13">
+        <v>59.7</v>
+      </c>
+      <c r="G13">
+        <v>59.7</v>
+      </c>
+      <c r="H13">
+        <v>60</v>
+      </c>
+      <c r="I13">
+        <v>60.5</v>
+      </c>
+      <c r="J13">
+        <v>61.2</v>
+      </c>
+      <c r="K13">
         <v>62</v>
       </c>
-      <c r="D13">
-        <v>60.5</v>
-      </c>
-      <c r="E13">
-        <v>59.1</v>
-      </c>
-      <c r="F13">
-        <v>57.6</v>
-      </c>
-      <c r="G13">
-        <v>56.3</v>
-      </c>
-      <c r="H13">
-        <v>55</v>
-      </c>
-      <c r="I13">
-        <v>53.9</v>
-      </c>
-      <c r="J13">
-        <v>53</v>
-      </c>
-      <c r="K13">
-        <v>52.2</v>
-      </c>
       <c r="L13">
-        <v>51.6</v>
+        <v>62.8</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -939,37 +939,37 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>58.3</v>
+        <v>58.9</v>
       </c>
       <c r="C14">
-        <v>58.2</v>
+        <v>60.2</v>
       </c>
       <c r="D14">
-        <v>58.6</v>
+        <v>62.6</v>
       </c>
       <c r="E14">
-        <v>59.7</v>
+        <v>65.90000000000001</v>
       </c>
       <c r="F14">
-        <v>61.4</v>
+        <v>70.2</v>
       </c>
       <c r="G14">
-        <v>63.7</v>
+        <v>75.40000000000001</v>
       </c>
       <c r="H14">
-        <v>66.5</v>
+        <v>81.3</v>
       </c>
       <c r="I14">
-        <v>69.8</v>
+        <v>87.5</v>
       </c>
       <c r="J14">
-        <v>73.40000000000001</v>
+        <v>93.90000000000001</v>
       </c>
       <c r="K14">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="L14">
-        <v>80.59999999999999</v>
+        <v>105.4</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -977,37 +977,37 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>64.8</v>
+        <v>62</v>
       </c>
       <c r="C15">
-        <v>61.7</v>
+        <v>59.3</v>
       </c>
       <c r="D15">
-        <v>58.6</v>
+        <v>56.8</v>
       </c>
       <c r="E15">
-        <v>55.6</v>
+        <v>54.9</v>
       </c>
       <c r="F15">
-        <v>52.9</v>
+        <v>53.6</v>
       </c>
       <c r="G15">
-        <v>50.8</v>
+        <v>53.2</v>
       </c>
       <c r="H15">
-        <v>49.4</v>
+        <v>53.8</v>
       </c>
       <c r="I15">
-        <v>48.8</v>
+        <v>55.2</v>
       </c>
       <c r="J15">
-        <v>49</v>
+        <v>57.4</v>
       </c>
       <c r="K15">
-        <v>50.1</v>
+        <v>60.3</v>
       </c>
       <c r="L15">
-        <v>51.8</v>
+        <v>63.5</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1015,37 +1015,37 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>56</v>
+        <v>55.2</v>
       </c>
       <c r="C16">
-        <v>54.9</v>
+        <v>54.4</v>
       </c>
       <c r="D16">
         <v>53.9</v>
       </c>
       <c r="E16">
-        <v>52.9</v>
+        <v>53.7</v>
       </c>
       <c r="F16">
-        <v>52.1</v>
+        <v>53.7</v>
       </c>
       <c r="G16">
-        <v>51.3</v>
+        <v>53.8</v>
       </c>
       <c r="H16">
-        <v>50.7</v>
+        <v>54.2</v>
       </c>
       <c r="I16">
-        <v>50.1</v>
+        <v>54.8</v>
       </c>
       <c r="J16">
-        <v>49.7</v>
+        <v>55.5</v>
       </c>
       <c r="K16">
-        <v>49.4</v>
+        <v>56.2</v>
       </c>
       <c r="L16">
-        <v>49.2</v>
+        <v>56.9</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1053,37 +1053,37 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>63.3</v>
+        <v>62.4</v>
       </c>
       <c r="C17">
-        <v>62.1</v>
+        <v>61.4</v>
       </c>
       <c r="D17">
-        <v>60.8</v>
+        <v>60.5</v>
       </c>
       <c r="E17">
-        <v>59.4</v>
+        <v>59.7</v>
       </c>
       <c r="F17">
-        <v>58.1</v>
+        <v>59.1</v>
       </c>
       <c r="G17">
-        <v>56.7</v>
+        <v>58.7</v>
       </c>
       <c r="H17">
-        <v>55.4</v>
+        <v>58.5</v>
       </c>
       <c r="I17">
-        <v>54.3</v>
+        <v>58.6</v>
       </c>
       <c r="J17">
-        <v>53.4</v>
+        <v>58.8</v>
       </c>
       <c r="K17">
-        <v>52.6</v>
+        <v>59.3</v>
       </c>
       <c r="L17">
-        <v>52.1</v>
+        <v>59.9</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1091,37 +1091,37 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>63.6</v>
+        <v>61.5</v>
       </c>
       <c r="C18">
-        <v>61.3</v>
+        <v>59.6</v>
       </c>
       <c r="D18">
-        <v>59.2</v>
+        <v>58</v>
       </c>
       <c r="E18">
-        <v>57.3</v>
+        <v>56.9</v>
       </c>
       <c r="F18">
-        <v>55.8</v>
+        <v>56.4</v>
       </c>
       <c r="G18">
-        <v>54.7</v>
+        <v>56.4</v>
       </c>
       <c r="H18">
-        <v>54.2</v>
+        <v>57.2</v>
       </c>
       <c r="I18">
-        <v>54.3</v>
+        <v>58.5</v>
       </c>
       <c r="J18">
-        <v>54.9</v>
+        <v>60.4</v>
       </c>
       <c r="K18">
-        <v>56.1</v>
+        <v>62.5</v>
       </c>
       <c r="L18">
-        <v>57.6</v>
+        <v>64.90000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1129,37 +1129,37 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>55.2</v>
+        <v>56.9</v>
       </c>
       <c r="C19">
-        <v>56.2</v>
+        <v>58.8</v>
       </c>
       <c r="D19">
-        <v>57.3</v>
+        <v>61.2</v>
       </c>
       <c r="E19">
-        <v>58.4</v>
+        <v>63.8</v>
       </c>
       <c r="F19">
-        <v>59.4</v>
+        <v>66.59999999999999</v>
       </c>
       <c r="G19">
-        <v>60.3</v>
+        <v>69.59999999999999</v>
       </c>
       <c r="H19">
-        <v>61</v>
+        <v>72.59999999999999</v>
       </c>
       <c r="I19">
-        <v>61.5</v>
+        <v>75.59999999999999</v>
       </c>
       <c r="J19">
-        <v>61.8</v>
+        <v>78.40000000000001</v>
       </c>
       <c r="K19">
-        <v>62</v>
+        <v>80.90000000000001</v>
       </c>
       <c r="L19">
-        <v>62</v>
+        <v>82.90000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1167,37 +1167,37 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>64.40000000000001</v>
+        <v>64.7</v>
       </c>
       <c r="C20">
-        <v>64.3</v>
+        <v>65</v>
       </c>
       <c r="D20">
-        <v>64.09999999999999</v>
+        <v>65.59999999999999</v>
       </c>
       <c r="E20">
-        <v>63.9</v>
+        <v>66.5</v>
       </c>
       <c r="F20">
-        <v>63.8</v>
+        <v>67.8</v>
       </c>
       <c r="G20">
-        <v>63.8</v>
+        <v>69.59999999999999</v>
       </c>
       <c r="H20">
-        <v>64.2</v>
+        <v>71.90000000000001</v>
       </c>
       <c r="I20">
-        <v>65</v>
+        <v>74.7</v>
       </c>
       <c r="J20">
-        <v>66.09999999999999</v>
+        <v>77.8</v>
       </c>
       <c r="K20">
-        <v>67.59999999999999</v>
+        <v>81</v>
       </c>
       <c r="L20">
-        <v>69.3</v>
+        <v>84.09999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1205,37 +1205,37 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>54</v>
+        <v>53.3</v>
       </c>
       <c r="C21">
-        <v>52.9</v>
+        <v>52.8</v>
       </c>
       <c r="D21">
-        <v>51.8</v>
+        <v>52.5</v>
       </c>
       <c r="E21">
-        <v>50.8</v>
+        <v>52.5</v>
       </c>
       <c r="F21">
-        <v>49.8</v>
+        <v>52.8</v>
       </c>
       <c r="G21">
-        <v>48.8</v>
+        <v>53.4</v>
       </c>
       <c r="H21">
-        <v>48</v>
+        <v>54.3</v>
       </c>
       <c r="I21">
-        <v>47.3</v>
+        <v>55.4</v>
       </c>
       <c r="J21">
-        <v>46.8</v>
+        <v>56.8</v>
       </c>
       <c r="K21">
-        <v>46.6</v>
+        <v>58.4</v>
       </c>
       <c r="L21">
-        <v>46.7</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to VIIRS version 2 data
</commit_message>
<xml_diff>
--- a/passage_clusters/VIIRS/CLUSTER_1/VCI3M_Forecast_Overview_CLUSTER_1.xlsx
+++ b/passage_clusters/VIIRS/CLUSTER_1/VCI3M_Forecast_Overview_CLUSTER_1.xlsx
@@ -445,37 +445,37 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="B1" s="1">
-        <v>45685</v>
+        <v>45727</v>
       </c>
       <c r="C1" s="1">
-        <v>45692</v>
+        <v>45734</v>
       </c>
       <c r="D1" s="1">
-        <v>45699</v>
+        <v>45741</v>
       </c>
       <c r="E1" s="1">
-        <v>45706</v>
+        <v>45748</v>
       </c>
       <c r="F1" s="1">
-        <v>45713</v>
+        <v>45755</v>
       </c>
       <c r="G1" s="1">
-        <v>45720</v>
+        <v>45762</v>
       </c>
       <c r="H1" s="1">
-        <v>45727</v>
+        <v>45769</v>
       </c>
       <c r="I1" s="1">
-        <v>45734</v>
+        <v>45776</v>
       </c>
       <c r="J1" s="1">
-        <v>45741</v>
+        <v>45783</v>
       </c>
       <c r="K1" s="1">
-        <v>45748</v>
+        <v>45790</v>
       </c>
       <c r="L1" s="1">
-        <v>45755</v>
+        <v>45797</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -483,37 +483,37 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>61.1</v>
+        <v>48.3</v>
       </c>
       <c r="C2">
-        <v>60.4</v>
+        <v>45.1</v>
       </c>
       <c r="D2">
-        <v>60</v>
+        <v>42.1</v>
       </c>
       <c r="E2">
-        <v>59.9</v>
+        <v>39.4</v>
       </c>
       <c r="F2">
-        <v>60.3</v>
+        <v>37.2</v>
       </c>
       <c r="G2">
-        <v>61</v>
+        <v>35.6</v>
       </c>
       <c r="H2">
-        <v>62.3</v>
+        <v>34.4</v>
       </c>
       <c r="I2">
-        <v>63.8</v>
+        <v>33.8</v>
       </c>
       <c r="J2">
-        <v>65.7</v>
+        <v>33.6</v>
       </c>
       <c r="K2">
-        <v>67.7</v>
+        <v>33.9</v>
       </c>
       <c r="L2">
-        <v>69.7</v>
+        <v>34.6</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -521,37 +521,37 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>64.09999999999999</v>
+        <v>65.59999999999999</v>
       </c>
       <c r="C3">
-        <v>65.90000000000001</v>
+        <v>63</v>
       </c>
       <c r="D3">
-        <v>67.7</v>
+        <v>59.6</v>
       </c>
       <c r="E3">
-        <v>69.59999999999999</v>
+        <v>55.6</v>
       </c>
       <c r="F3">
-        <v>71.5</v>
+        <v>51</v>
       </c>
       <c r="G3">
-        <v>73.3</v>
+        <v>46.3</v>
       </c>
       <c r="H3">
-        <v>75</v>
+        <v>41.6</v>
       </c>
       <c r="I3">
-        <v>76.40000000000001</v>
+        <v>37.2</v>
       </c>
       <c r="J3">
-        <v>77.59999999999999</v>
+        <v>33.3</v>
       </c>
       <c r="K3">
-        <v>78.5</v>
+        <v>30.1</v>
       </c>
       <c r="L3">
-        <v>78.90000000000001</v>
+        <v>27.8</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -559,37 +559,37 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>42.5</v>
+        <v>30.2</v>
       </c>
       <c r="C4">
-        <v>41.8</v>
+        <v>26.3</v>
       </c>
       <c r="D4">
-        <v>41.5</v>
+        <v>22.6</v>
       </c>
       <c r="E4">
-        <v>41.6</v>
+        <v>19.3</v>
       </c>
       <c r="F4">
-        <v>42.3</v>
+        <v>16.7</v>
       </c>
       <c r="G4">
-        <v>43.6</v>
+        <v>14.7</v>
       </c>
       <c r="H4">
-        <v>45.4</v>
+        <v>13.3</v>
       </c>
       <c r="I4">
-        <v>47.7</v>
+        <v>12.5</v>
       </c>
       <c r="J4">
-        <v>50.4</v>
+        <v>12.3</v>
       </c>
       <c r="K4">
-        <v>53.3</v>
+        <v>12.8</v>
       </c>
       <c r="L4">
-        <v>56.3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -597,37 +597,37 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>64.2</v>
+        <v>47.7</v>
       </c>
       <c r="C5">
-        <v>62.6</v>
+        <v>44.2</v>
       </c>
       <c r="D5">
-        <v>61.2</v>
+        <v>41</v>
       </c>
       <c r="E5">
-        <v>60.2</v>
+        <v>38.2</v>
       </c>
       <c r="F5">
-        <v>59.5</v>
+        <v>36</v>
       </c>
       <c r="G5">
-        <v>59.2</v>
+        <v>34.2</v>
       </c>
       <c r="H5">
-        <v>59.4</v>
+        <v>32.9</v>
       </c>
       <c r="I5">
-        <v>60</v>
+        <v>32.1</v>
       </c>
       <c r="J5">
-        <v>61</v>
+        <v>31.8</v>
       </c>
       <c r="K5">
-        <v>62.2</v>
+        <v>31.9</v>
       </c>
       <c r="L5">
-        <v>63.6</v>
+        <v>32.4</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -635,37 +635,37 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>64.59999999999999</v>
+        <v>66.2</v>
       </c>
       <c r="C6">
-        <v>66.7</v>
+        <v>64.2</v>
       </c>
       <c r="D6">
-        <v>68.90000000000001</v>
+        <v>62.1</v>
       </c>
       <c r="E6">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="F6">
-        <v>73</v>
+        <v>58.2</v>
       </c>
       <c r="G6">
-        <v>74.7</v>
+        <v>56.9</v>
       </c>
       <c r="H6">
-        <v>76.2</v>
+        <v>56</v>
       </c>
       <c r="I6">
-        <v>77.3</v>
+        <v>55.7</v>
       </c>
       <c r="J6">
-        <v>78.2</v>
+        <v>55.7</v>
       </c>
       <c r="K6">
-        <v>78.7</v>
+        <v>56.1</v>
       </c>
       <c r="L6">
-        <v>78.90000000000001</v>
+        <v>56.6</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -673,37 +673,37 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>60.4</v>
+        <v>42.2</v>
       </c>
       <c r="C7">
-        <v>59.9</v>
+        <v>39.9</v>
       </c>
       <c r="D7">
-        <v>59.7</v>
+        <v>38.3</v>
       </c>
       <c r="E7">
-        <v>59.7</v>
+        <v>37.4</v>
       </c>
       <c r="F7">
-        <v>60.2</v>
+        <v>37.5</v>
       </c>
       <c r="G7">
-        <v>61.3</v>
+        <v>38.2</v>
       </c>
       <c r="H7">
-        <v>62.9</v>
+        <v>39.6</v>
       </c>
       <c r="I7">
-        <v>65.09999999999999</v>
+        <v>41.5</v>
       </c>
       <c r="J7">
-        <v>67.59999999999999</v>
+        <v>43.7</v>
       </c>
       <c r="K7">
-        <v>70.40000000000001</v>
+        <v>46.1</v>
       </c>
       <c r="L7">
-        <v>73.2</v>
+        <v>48.4</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -711,37 +711,37 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>68.59999999999999</v>
+        <v>52.2</v>
       </c>
       <c r="C8">
-        <v>67.09999999999999</v>
+        <v>48.7</v>
       </c>
       <c r="D8">
-        <v>65.8</v>
+        <v>45.5</v>
       </c>
       <c r="E8">
-        <v>65</v>
+        <v>42.7</v>
       </c>
       <c r="F8">
-        <v>64.59999999999999</v>
+        <v>40.6</v>
       </c>
       <c r="G8">
-        <v>64.7</v>
+        <v>39.1</v>
       </c>
       <c r="H8">
-        <v>65.3</v>
+        <v>38.1</v>
       </c>
       <c r="I8">
-        <v>66.40000000000001</v>
+        <v>37.7</v>
       </c>
       <c r="J8">
-        <v>68</v>
+        <v>37.7</v>
       </c>
       <c r="K8">
-        <v>69.90000000000001</v>
+        <v>38.2</v>
       </c>
       <c r="L8">
-        <v>71.90000000000001</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -749,37 +749,37 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>60.8</v>
+        <v>39</v>
       </c>
       <c r="C9">
-        <v>58.7</v>
+        <v>36</v>
       </c>
       <c r="D9">
-        <v>57.1</v>
+        <v>33.7</v>
       </c>
       <c r="E9">
-        <v>56.1</v>
+        <v>32.1</v>
       </c>
       <c r="F9">
-        <v>55.8</v>
+        <v>31.2</v>
       </c>
       <c r="G9">
-        <v>56.4</v>
+        <v>31</v>
       </c>
       <c r="H9">
-        <v>57.8</v>
+        <v>31.4</v>
       </c>
       <c r="I9">
-        <v>60.1</v>
+        <v>32.3</v>
       </c>
       <c r="J9">
-        <v>62.9</v>
+        <v>33.7</v>
       </c>
       <c r="K9">
-        <v>66.09999999999999</v>
+        <v>35.5</v>
       </c>
       <c r="L9">
-        <v>69.5</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -787,37 +787,37 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>60.7</v>
+        <v>36.9</v>
       </c>
       <c r="C10">
-        <v>57.9</v>
+        <v>34.4</v>
       </c>
       <c r="D10">
-        <v>55.5</v>
+        <v>32.7</v>
       </c>
       <c r="E10">
-        <v>53.8</v>
+        <v>31.9</v>
       </c>
       <c r="F10">
-        <v>52.9</v>
+        <v>32</v>
       </c>
       <c r="G10">
-        <v>52.7</v>
+        <v>32.7</v>
       </c>
       <c r="H10">
-        <v>53.4</v>
+        <v>34.1</v>
       </c>
       <c r="I10">
-        <v>54.8</v>
+        <v>36</v>
       </c>
       <c r="J10">
-        <v>56.8</v>
+        <v>38.2</v>
       </c>
       <c r="K10">
-        <v>59.3</v>
+        <v>40.6</v>
       </c>
       <c r="L10">
-        <v>62</v>
+        <v>43.1</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -825,37 +825,37 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>72.59999999999999</v>
+        <v>52.3</v>
       </c>
       <c r="C11">
-        <v>70.40000000000001</v>
+        <v>48.7</v>
       </c>
       <c r="D11">
-        <v>68.5</v>
+        <v>45.5</v>
       </c>
       <c r="E11">
-        <v>67</v>
+        <v>42.9</v>
       </c>
       <c r="F11">
-        <v>66.09999999999999</v>
+        <v>41</v>
       </c>
       <c r="G11">
-        <v>65.90000000000001</v>
+        <v>39.7</v>
       </c>
       <c r="H11">
-        <v>66.3</v>
+        <v>38.8</v>
       </c>
       <c r="I11">
-        <v>67.40000000000001</v>
+        <v>38.6</v>
       </c>
       <c r="J11">
-        <v>69.09999999999999</v>
+        <v>38.8</v>
       </c>
       <c r="K11">
-        <v>71.09999999999999</v>
+        <v>39.4</v>
       </c>
       <c r="L11">
-        <v>73.3</v>
+        <v>40.4</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -863,37 +863,37 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>65.3</v>
+        <v>56.6</v>
       </c>
       <c r="C12">
-        <v>63.8</v>
+        <v>53</v>
       </c>
       <c r="D12">
-        <v>62.3</v>
+        <v>49.5</v>
       </c>
       <c r="E12">
-        <v>60.9</v>
+        <v>46.3</v>
       </c>
       <c r="F12">
-        <v>59.5</v>
+        <v>43.5</v>
       </c>
       <c r="G12">
-        <v>58.3</v>
+        <v>41.2</v>
       </c>
       <c r="H12">
-        <v>57.3</v>
+        <v>39.2</v>
       </c>
       <c r="I12">
-        <v>56.5</v>
+        <v>37.8</v>
       </c>
       <c r="J12">
-        <v>55.9</v>
+        <v>36.7</v>
       </c>
       <c r="K12">
-        <v>55.6</v>
+        <v>36.1</v>
       </c>
       <c r="L12">
-        <v>55.4</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -901,37 +901,37 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>62.3</v>
+        <v>59.1</v>
       </c>
       <c r="C13">
-        <v>61.4</v>
+        <v>56.4</v>
       </c>
       <c r="D13">
-        <v>60.6</v>
+        <v>53.7</v>
       </c>
       <c r="E13">
-        <v>60</v>
+        <v>50.9</v>
       </c>
       <c r="F13">
-        <v>59.7</v>
+        <v>48.3</v>
       </c>
       <c r="G13">
-        <v>59.7</v>
+        <v>46</v>
       </c>
       <c r="H13">
-        <v>60</v>
+        <v>43.8</v>
       </c>
       <c r="I13">
-        <v>60.5</v>
+        <v>42</v>
       </c>
       <c r="J13">
-        <v>61.2</v>
+        <v>40.6</v>
       </c>
       <c r="K13">
-        <v>62</v>
+        <v>39.6</v>
       </c>
       <c r="L13">
-        <v>62.8</v>
+        <v>39.1</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -939,37 +939,37 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>58.9</v>
+        <v>43.7</v>
       </c>
       <c r="C14">
-        <v>60.2</v>
+        <v>41</v>
       </c>
       <c r="D14">
-        <v>62.6</v>
+        <v>38.4</v>
       </c>
       <c r="E14">
-        <v>65.90000000000001</v>
+        <v>36.2</v>
       </c>
       <c r="F14">
-        <v>70.2</v>
+        <v>34.4</v>
       </c>
       <c r="G14">
-        <v>75.40000000000001</v>
+        <v>33.1</v>
       </c>
       <c r="H14">
-        <v>81.3</v>
+        <v>32.3</v>
       </c>
       <c r="I14">
-        <v>87.5</v>
+        <v>32</v>
       </c>
       <c r="J14">
-        <v>93.90000000000001</v>
+        <v>32.1</v>
       </c>
       <c r="K14">
-        <v>100</v>
+        <v>32.6</v>
       </c>
       <c r="L14">
-        <v>105.4</v>
+        <v>33.4</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -977,37 +977,37 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>62</v>
+        <v>37.9</v>
       </c>
       <c r="C15">
-        <v>59.3</v>
+        <v>34</v>
       </c>
       <c r="D15">
-        <v>56.8</v>
+        <v>30.6</v>
       </c>
       <c r="E15">
-        <v>54.9</v>
+        <v>27.8</v>
       </c>
       <c r="F15">
-        <v>53.6</v>
+        <v>25.6</v>
       </c>
       <c r="G15">
-        <v>53.2</v>
+        <v>23.9</v>
       </c>
       <c r="H15">
-        <v>53.8</v>
+        <v>22.7</v>
       </c>
       <c r="I15">
-        <v>55.2</v>
+        <v>21.8</v>
       </c>
       <c r="J15">
-        <v>57.4</v>
+        <v>21.2</v>
       </c>
       <c r="K15">
-        <v>60.3</v>
+        <v>21</v>
       </c>
       <c r="L15">
-        <v>63.5</v>
+        <v>21.2</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1015,37 +1015,37 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>55.2</v>
+        <v>48.6</v>
       </c>
       <c r="C16">
-        <v>54.4</v>
+        <v>44.8</v>
       </c>
       <c r="D16">
-        <v>53.9</v>
+        <v>40.8</v>
       </c>
       <c r="E16">
-        <v>53.7</v>
+        <v>37</v>
       </c>
       <c r="F16">
-        <v>53.7</v>
+        <v>33.4</v>
       </c>
       <c r="G16">
-        <v>53.8</v>
+        <v>30.1</v>
       </c>
       <c r="H16">
-        <v>54.2</v>
+        <v>27.2</v>
       </c>
       <c r="I16">
-        <v>54.8</v>
+        <v>24.8</v>
       </c>
       <c r="J16">
-        <v>55.5</v>
+        <v>23</v>
       </c>
       <c r="K16">
-        <v>56.2</v>
+        <v>21.9</v>
       </c>
       <c r="L16">
-        <v>56.9</v>
+        <v>21.4</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1053,37 +1053,37 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>62.4</v>
+        <v>55</v>
       </c>
       <c r="C17">
-        <v>61.4</v>
+        <v>50.9</v>
       </c>
       <c r="D17">
-        <v>60.5</v>
+        <v>46.7</v>
       </c>
       <c r="E17">
-        <v>59.7</v>
+        <v>42.6</v>
       </c>
       <c r="F17">
-        <v>59.1</v>
+        <v>38.7</v>
       </c>
       <c r="G17">
-        <v>58.7</v>
+        <v>35.3</v>
       </c>
       <c r="H17">
-        <v>58.5</v>
+        <v>32.3</v>
       </c>
       <c r="I17">
-        <v>58.6</v>
+        <v>29.9</v>
       </c>
       <c r="J17">
-        <v>58.8</v>
+        <v>28.1</v>
       </c>
       <c r="K17">
-        <v>59.3</v>
+        <v>27</v>
       </c>
       <c r="L17">
-        <v>59.9</v>
+        <v>26.7</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1091,37 +1091,37 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>61.5</v>
+        <v>42.3</v>
       </c>
       <c r="C18">
-        <v>59.6</v>
+        <v>38.6</v>
       </c>
       <c r="D18">
-        <v>58</v>
+        <v>35.3</v>
       </c>
       <c r="E18">
-        <v>56.9</v>
+        <v>32.4</v>
       </c>
       <c r="F18">
-        <v>56.4</v>
+        <v>30.1</v>
       </c>
       <c r="G18">
-        <v>56.4</v>
+        <v>28.3</v>
       </c>
       <c r="H18">
-        <v>57.2</v>
+        <v>27.1</v>
       </c>
       <c r="I18">
-        <v>58.5</v>
+        <v>26.4</v>
       </c>
       <c r="J18">
-        <v>60.4</v>
+        <v>26.3</v>
       </c>
       <c r="K18">
-        <v>62.5</v>
+        <v>26.7</v>
       </c>
       <c r="L18">
-        <v>64.90000000000001</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1129,37 +1129,37 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>56.9</v>
+        <v>53.9</v>
       </c>
       <c r="C19">
-        <v>58.8</v>
+        <v>51.3</v>
       </c>
       <c r="D19">
-        <v>61.2</v>
+        <v>48.7</v>
       </c>
       <c r="E19">
-        <v>63.8</v>
+        <v>46.4</v>
       </c>
       <c r="F19">
-        <v>66.59999999999999</v>
+        <v>44.5</v>
       </c>
       <c r="G19">
-        <v>69.59999999999999</v>
+        <v>43.2</v>
       </c>
       <c r="H19">
-        <v>72.59999999999999</v>
+        <v>42.6</v>
       </c>
       <c r="I19">
-        <v>75.59999999999999</v>
+        <v>42.7</v>
       </c>
       <c r="J19">
-        <v>78.40000000000001</v>
+        <v>43.2</v>
       </c>
       <c r="K19">
-        <v>80.90000000000001</v>
+        <v>44.2</v>
       </c>
       <c r="L19">
-        <v>82.90000000000001</v>
+        <v>45.4</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1167,37 +1167,37 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>64.7</v>
+        <v>46.8</v>
       </c>
       <c r="C20">
-        <v>65</v>
+        <v>43.3</v>
       </c>
       <c r="D20">
-        <v>65.59999999999999</v>
+        <v>40.2</v>
       </c>
       <c r="E20">
-        <v>66.5</v>
+        <v>37.7</v>
       </c>
       <c r="F20">
-        <v>67.8</v>
+        <v>36</v>
       </c>
       <c r="G20">
-        <v>69.59999999999999</v>
+        <v>35.1</v>
       </c>
       <c r="H20">
-        <v>71.90000000000001</v>
+        <v>35.1</v>
       </c>
       <c r="I20">
-        <v>74.7</v>
+        <v>35.8</v>
       </c>
       <c r="J20">
-        <v>77.8</v>
+        <v>37.2</v>
       </c>
       <c r="K20">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="L20">
-        <v>84.09999999999999</v>
+        <v>41.2</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1205,37 +1205,37 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>53.3</v>
+        <v>42</v>
       </c>
       <c r="C21">
-        <v>52.8</v>
+        <v>38.3</v>
       </c>
       <c r="D21">
-        <v>52.5</v>
+        <v>34.7</v>
       </c>
       <c r="E21">
-        <v>52.5</v>
+        <v>31.5</v>
       </c>
       <c r="F21">
-        <v>52.8</v>
+        <v>29</v>
       </c>
       <c r="G21">
-        <v>53.4</v>
+        <v>27</v>
       </c>
       <c r="H21">
-        <v>54.3</v>
+        <v>25.7</v>
       </c>
       <c r="I21">
-        <v>55.4</v>
+        <v>25.1</v>
       </c>
       <c r="J21">
-        <v>56.8</v>
+        <v>25</v>
       </c>
       <c r="K21">
-        <v>58.4</v>
+        <v>25.6</v>
       </c>
       <c r="L21">
-        <v>60</v>
+        <v>26.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
early june 2025 update
</commit_message>
<xml_diff>
--- a/passage_clusters/VIIRS/CLUSTER_1/VCI3M_Forecast_Overview_CLUSTER_1.xlsx
+++ b/passage_clusters/VIIRS/CLUSTER_1/VCI3M_Forecast_Overview_CLUSTER_1.xlsx
@@ -445,37 +445,37 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="B1" s="1">
-        <v>45783</v>
+        <v>45797</v>
       </c>
       <c r="C1" s="1">
-        <v>45790</v>
+        <v>45804</v>
       </c>
       <c r="D1" s="1">
-        <v>45797</v>
+        <v>45811</v>
       </c>
       <c r="E1" s="1">
-        <v>45804</v>
+        <v>45818</v>
       </c>
       <c r="F1" s="1">
-        <v>45811</v>
+        <v>45825</v>
       </c>
       <c r="G1" s="1">
-        <v>45818</v>
+        <v>45832</v>
       </c>
       <c r="H1" s="1">
-        <v>45825</v>
+        <v>45839</v>
       </c>
       <c r="I1" s="1">
-        <v>45832</v>
+        <v>45846</v>
       </c>
       <c r="J1" s="1">
-        <v>45839</v>
+        <v>45853</v>
       </c>
       <c r="K1" s="1">
-        <v>45846</v>
+        <v>45860</v>
       </c>
       <c r="L1" s="1">
-        <v>45853</v>
+        <v>45867</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -483,37 +483,37 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>54.8</v>
+        <v>61.8</v>
       </c>
       <c r="C2">
-        <v>58.2</v>
+        <v>64.8</v>
       </c>
       <c r="D2">
-        <v>61.2</v>
+        <v>67</v>
       </c>
       <c r="E2">
-        <v>63.6</v>
+        <v>68.3</v>
       </c>
       <c r="F2">
-        <v>65</v>
+        <v>68.7</v>
       </c>
       <c r="G2">
-        <v>65.40000000000001</v>
+        <v>68.09999999999999</v>
       </c>
       <c r="H2">
-        <v>64.59999999999999</v>
+        <v>66.59999999999999</v>
       </c>
       <c r="I2">
-        <v>62.7</v>
+        <v>64.40000000000001</v>
       </c>
       <c r="J2">
-        <v>59.8</v>
+        <v>61.8</v>
       </c>
       <c r="K2">
-        <v>56.1</v>
+        <v>58.8</v>
       </c>
       <c r="L2">
-        <v>52</v>
+        <v>55.9</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -521,37 +521,37 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>65.2</v>
+        <v>69.2</v>
       </c>
       <c r="C3">
-        <v>67.3</v>
+        <v>70.7</v>
       </c>
       <c r="D3">
-        <v>69.2</v>
+        <v>71.40000000000001</v>
       </c>
       <c r="E3">
-        <v>70.7</v>
+        <v>71.3</v>
       </c>
       <c r="F3">
-        <v>71.5</v>
+        <v>70</v>
       </c>
       <c r="G3">
-        <v>71.40000000000001</v>
+        <v>67.5</v>
       </c>
       <c r="H3">
-        <v>70.09999999999999</v>
+        <v>64</v>
       </c>
       <c r="I3">
-        <v>67.7</v>
+        <v>59.7</v>
       </c>
       <c r="J3">
-        <v>64.3</v>
+        <v>54.8</v>
       </c>
       <c r="K3">
-        <v>59.9</v>
+        <v>49.7</v>
       </c>
       <c r="L3">
-        <v>55.1</v>
+        <v>44.9</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -559,37 +559,37 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>32.8</v>
+        <v>38.9</v>
       </c>
       <c r="C4">
-        <v>35.9</v>
+        <v>41.2</v>
       </c>
       <c r="D4">
-        <v>38.6</v>
+        <v>42.5</v>
       </c>
       <c r="E4">
-        <v>40.4</v>
+        <v>42.8</v>
       </c>
       <c r="F4">
-        <v>41.2</v>
+        <v>41.9</v>
       </c>
       <c r="G4">
-        <v>40.7</v>
+        <v>39.9</v>
       </c>
       <c r="H4">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I4">
-        <v>35.9</v>
+        <v>33.4</v>
       </c>
       <c r="J4">
-        <v>31.9</v>
+        <v>29.5</v>
       </c>
       <c r="K4">
-        <v>27.1</v>
+        <v>25.7</v>
       </c>
       <c r="L4">
-        <v>22.1</v>
+        <v>22.4</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -597,37 +597,37 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>59.9</v>
+        <v>68.40000000000001</v>
       </c>
       <c r="C5">
-        <v>64.09999999999999</v>
+        <v>72</v>
       </c>
       <c r="D5">
-        <v>67.8</v>
+        <v>74.59999999999999</v>
       </c>
       <c r="E5">
-        <v>70.59999999999999</v>
+        <v>76.3</v>
       </c>
       <c r="F5">
-        <v>72.3</v>
+        <v>76.8</v>
       </c>
       <c r="G5">
-        <v>72.8</v>
+        <v>76.2</v>
       </c>
       <c r="H5">
-        <v>71.90000000000001</v>
+        <v>74.7</v>
       </c>
       <c r="I5">
-        <v>69.7</v>
+        <v>72.2</v>
       </c>
       <c r="J5">
-        <v>66.3</v>
+        <v>69.3</v>
       </c>
       <c r="K5">
-        <v>62.1</v>
+        <v>66</v>
       </c>
       <c r="L5">
-        <v>57.3</v>
+        <v>62.7</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -635,37 +635,37 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>71</v>
+        <v>75.5</v>
       </c>
       <c r="C6">
-        <v>72.7</v>
+        <v>77.40000000000001</v>
       </c>
       <c r="D6">
-        <v>73.8</v>
+        <v>78.7</v>
       </c>
       <c r="E6">
-        <v>73.90000000000001</v>
+        <v>79.40000000000001</v>
       </c>
       <c r="F6">
-        <v>73</v>
+        <v>79.59999999999999</v>
       </c>
       <c r="G6">
-        <v>71</v>
+        <v>79.2</v>
       </c>
       <c r="H6">
-        <v>67.8</v>
+        <v>78.3</v>
       </c>
       <c r="I6">
-        <v>63.7</v>
+        <v>77.2</v>
       </c>
       <c r="J6">
-        <v>58.9</v>
+        <v>75.90000000000001</v>
       </c>
       <c r="K6">
-        <v>53.7</v>
+        <v>74.5</v>
       </c>
       <c r="L6">
-        <v>48.5</v>
+        <v>73.09999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -673,37 +673,37 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>55.9</v>
+        <v>63.4</v>
       </c>
       <c r="C7">
-        <v>59.5</v>
+        <v>66.40000000000001</v>
       </c>
       <c r="D7">
-        <v>62.4</v>
+        <v>68.59999999999999</v>
       </c>
       <c r="E7">
-        <v>64.5</v>
+        <v>70</v>
       </c>
       <c r="F7">
-        <v>65.5</v>
+        <v>70.5</v>
       </c>
       <c r="G7">
-        <v>65.40000000000001</v>
+        <v>70.3</v>
       </c>
       <c r="H7">
+        <v>69.3</v>
+      </c>
+      <c r="I7">
+        <v>67.90000000000001</v>
+      </c>
+      <c r="J7">
+        <v>66.09999999999999</v>
+      </c>
+      <c r="K7">
         <v>64.09999999999999</v>
       </c>
-      <c r="I7">
-        <v>61.8</v>
-      </c>
-      <c r="J7">
-        <v>58.7</v>
-      </c>
-      <c r="K7">
-        <v>55</v>
-      </c>
       <c r="L7">
-        <v>51.1</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -711,37 +711,37 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>62.6</v>
+        <v>70.90000000000001</v>
       </c>
       <c r="C8">
-        <v>66.7</v>
+        <v>74.3</v>
       </c>
       <c r="D8">
-        <v>70.2</v>
+        <v>76.7</v>
       </c>
       <c r="E8">
-        <v>72.90000000000001</v>
+        <v>78</v>
       </c>
       <c r="F8">
-        <v>74.5</v>
+        <v>78.09999999999999</v>
       </c>
       <c r="G8">
-        <v>74.7</v>
+        <v>77</v>
       </c>
       <c r="H8">
-        <v>73.40000000000001</v>
+        <v>74.8</v>
       </c>
       <c r="I8">
-        <v>70.8</v>
+        <v>71.8</v>
       </c>
       <c r="J8">
-        <v>67</v>
+        <v>68.2</v>
       </c>
       <c r="K8">
-        <v>62.2</v>
+        <v>64.3</v>
       </c>
       <c r="L8">
-        <v>57</v>
+        <v>60.5</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -749,37 +749,37 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>53.5</v>
+        <v>61.1</v>
       </c>
       <c r="C9">
-        <v>57.2</v>
+        <v>64.09999999999999</v>
       </c>
       <c r="D9">
-        <v>60.4</v>
+        <v>66.40000000000001</v>
       </c>
       <c r="E9">
-        <v>62.7</v>
+        <v>67.8</v>
       </c>
       <c r="F9">
-        <v>64</v>
+        <v>68.3</v>
       </c>
       <c r="G9">
-        <v>64.2</v>
+        <v>68</v>
       </c>
       <c r="H9">
+        <v>66.90000000000001</v>
+      </c>
+      <c r="I9">
+        <v>65.3</v>
+      </c>
+      <c r="J9">
         <v>63.3</v>
       </c>
-      <c r="I9">
-        <v>61.3</v>
-      </c>
-      <c r="J9">
-        <v>58.5</v>
-      </c>
       <c r="K9">
-        <v>55</v>
+        <v>61.2</v>
       </c>
       <c r="L9">
-        <v>51.3</v>
+        <v>59.2</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -787,37 +787,37 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>46.8</v>
+        <v>52.4</v>
       </c>
       <c r="C10">
-        <v>49.7</v>
+        <v>54.5</v>
       </c>
       <c r="D10">
-        <v>52</v>
+        <v>55.9</v>
       </c>
       <c r="E10">
-        <v>53.8</v>
+        <v>56.8</v>
       </c>
       <c r="F10">
-        <v>54.7</v>
+        <v>56.9</v>
       </c>
       <c r="G10">
-        <v>54.8</v>
+        <v>56.4</v>
       </c>
       <c r="H10">
+        <v>55.5</v>
+      </c>
+      <c r="I10">
         <v>54.2</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>52.8</v>
       </c>
-      <c r="J10">
-        <v>50.8</v>
-      </c>
       <c r="K10">
-        <v>48.5</v>
+        <v>51.3</v>
       </c>
       <c r="L10">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -825,37 +825,37 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>63.1</v>
+        <v>69.90000000000001</v>
       </c>
       <c r="C11">
-        <v>65.90000000000001</v>
+        <v>72.7</v>
       </c>
       <c r="D11">
-        <v>68</v>
+        <v>75.09999999999999</v>
       </c>
       <c r="E11">
-        <v>69.09999999999999</v>
+        <v>77</v>
       </c>
       <c r="F11">
-        <v>69.09999999999999</v>
+        <v>78.2</v>
       </c>
       <c r="G11">
-        <v>67.90000000000001</v>
+        <v>78.8</v>
       </c>
       <c r="H11">
-        <v>65.5</v>
+        <v>79</v>
       </c>
       <c r="I11">
-        <v>62</v>
+        <v>78.7</v>
       </c>
       <c r="J11">
-        <v>57.8</v>
+        <v>78.3</v>
       </c>
       <c r="K11">
-        <v>53.1</v>
+        <v>77.59999999999999</v>
       </c>
       <c r="L11">
-        <v>48.3</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -863,37 +863,37 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>62.5</v>
+        <v>70</v>
       </c>
       <c r="C12">
-        <v>66.2</v>
+        <v>73.3</v>
       </c>
       <c r="D12">
-        <v>69.8</v>
+        <v>75.8</v>
       </c>
       <c r="E12">
+        <v>77.3</v>
+      </c>
+      <c r="F12">
+        <v>77.8</v>
+      </c>
+      <c r="G12">
+        <v>77.09999999999999</v>
+      </c>
+      <c r="H12">
+        <v>75.40000000000001</v>
+      </c>
+      <c r="I12">
         <v>72.8</v>
       </c>
-      <c r="F12">
-        <v>74.90000000000001</v>
-      </c>
-      <c r="G12">
-        <v>75.90000000000001</v>
-      </c>
-      <c r="H12">
-        <v>75.8</v>
-      </c>
-      <c r="I12">
-        <v>74.5</v>
-      </c>
       <c r="J12">
-        <v>72.09999999999999</v>
+        <v>69.5</v>
       </c>
       <c r="K12">
-        <v>68.8</v>
+        <v>65.8</v>
       </c>
       <c r="L12">
-        <v>64.90000000000001</v>
+        <v>62.1</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -901,37 +901,37 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>65.7</v>
+        <v>72.09999999999999</v>
       </c>
       <c r="C13">
-        <v>69.09999999999999</v>
+        <v>74.59999999999999</v>
       </c>
       <c r="D13">
-        <v>72.2</v>
+        <v>76.2</v>
       </c>
       <c r="E13">
-        <v>74.7</v>
+        <v>76.7</v>
       </c>
       <c r="F13">
-        <v>76.3</v>
+        <v>75.90000000000001</v>
       </c>
       <c r="G13">
-        <v>76.8</v>
+        <v>73.90000000000001</v>
       </c>
       <c r="H13">
-        <v>76.09999999999999</v>
+        <v>70.59999999999999</v>
       </c>
       <c r="I13">
-        <v>74.09999999999999</v>
+        <v>66.5</v>
       </c>
       <c r="J13">
-        <v>70.90000000000001</v>
+        <v>61.6</v>
       </c>
       <c r="K13">
-        <v>66.7</v>
+        <v>56.5</v>
       </c>
       <c r="L13">
-        <v>61.9</v>
+        <v>51.5</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -939,37 +939,37 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>44.8</v>
+        <v>50.2</v>
       </c>
       <c r="C14">
+        <v>52.6</v>
+      </c>
+      <c r="D14">
+        <v>54.6</v>
+      </c>
+      <c r="E14">
+        <v>56</v>
+      </c>
+      <c r="F14">
+        <v>56.7</v>
+      </c>
+      <c r="G14">
+        <v>56.6</v>
+      </c>
+      <c r="H14">
+        <v>55.7</v>
+      </c>
+      <c r="I14">
+        <v>54.2</v>
+      </c>
+      <c r="J14">
+        <v>52.2</v>
+      </c>
+      <c r="K14">
+        <v>49.9</v>
+      </c>
+      <c r="L14">
         <v>47.5</v>
-      </c>
-      <c r="D14">
-        <v>50.2</v>
-      </c>
-      <c r="E14">
-        <v>52.7</v>
-      </c>
-      <c r="F14">
-        <v>54.7</v>
-      </c>
-      <c r="G14">
-        <v>56.2</v>
-      </c>
-      <c r="H14">
-        <v>57</v>
-      </c>
-      <c r="I14">
-        <v>57</v>
-      </c>
-      <c r="J14">
-        <v>56.3</v>
-      </c>
-      <c r="K14">
-        <v>55</v>
-      </c>
-      <c r="L14">
-        <v>53.2</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -977,37 +977,37 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>39.1</v>
+        <v>46.9</v>
       </c>
       <c r="C15">
-        <v>43.1</v>
+        <v>50.7</v>
       </c>
       <c r="D15">
-        <v>47.2</v>
+        <v>54.1</v>
       </c>
       <c r="E15">
-        <v>51.3</v>
+        <v>56.9</v>
       </c>
       <c r="F15">
-        <v>55.1</v>
+        <v>58.9</v>
       </c>
       <c r="G15">
-        <v>58.4</v>
+        <v>59.9</v>
       </c>
       <c r="H15">
-        <v>61</v>
+        <v>59.9</v>
       </c>
       <c r="I15">
-        <v>62.7</v>
+        <v>59</v>
       </c>
       <c r="J15">
-        <v>63.4</v>
+        <v>57.1</v>
       </c>
       <c r="K15">
-        <v>63.2</v>
+        <v>54.7</v>
       </c>
       <c r="L15">
-        <v>62.1</v>
+        <v>51.8</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1015,37 +1015,37 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>51.4</v>
+        <v>59.2</v>
       </c>
       <c r="C16">
-        <v>55.3</v>
+        <v>62.5</v>
       </c>
       <c r="D16">
-        <v>59.1</v>
+        <v>64.90000000000001</v>
       </c>
       <c r="E16">
-        <v>62.4</v>
+        <v>66.2</v>
       </c>
       <c r="F16">
-        <v>64.7</v>
+        <v>66.09999999999999</v>
       </c>
       <c r="G16">
-        <v>65.7</v>
+        <v>64.5</v>
       </c>
       <c r="H16">
-        <v>65.40000000000001</v>
+        <v>61.7</v>
       </c>
       <c r="I16">
-        <v>63.6</v>
+        <v>57.8</v>
       </c>
       <c r="J16">
-        <v>60.5</v>
+        <v>53.1</v>
       </c>
       <c r="K16">
-        <v>56.3</v>
+        <v>48.1</v>
       </c>
       <c r="L16">
-        <v>51.3</v>
+        <v>43.2</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1053,37 +1053,37 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>52.6</v>
+        <v>59.6</v>
       </c>
       <c r="C17">
-        <v>56.2</v>
+        <v>62.9</v>
       </c>
       <c r="D17">
-        <v>60</v>
+        <v>65.40000000000001</v>
       </c>
       <c r="E17">
-        <v>63.5</v>
+        <v>67</v>
       </c>
       <c r="F17">
-        <v>66.5</v>
+        <v>67.3</v>
       </c>
       <c r="G17">
-        <v>68.5</v>
+        <v>66.3</v>
       </c>
       <c r="H17">
-        <v>69.5</v>
+        <v>64.09999999999999</v>
       </c>
       <c r="I17">
-        <v>69.2</v>
+        <v>60.7</v>
       </c>
       <c r="J17">
-        <v>67.59999999999999</v>
+        <v>56.5</v>
       </c>
       <c r="K17">
-        <v>65</v>
+        <v>51.8</v>
       </c>
       <c r="L17">
-        <v>61.4</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1091,37 +1091,37 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>56.8</v>
+        <v>65.40000000000001</v>
       </c>
       <c r="C18">
-        <v>60.8</v>
+        <v>68.8</v>
       </c>
       <c r="D18">
-        <v>64.09999999999999</v>
+        <v>71.3</v>
       </c>
       <c r="E18">
-        <v>66.2</v>
+        <v>72.90000000000001</v>
       </c>
       <c r="F18">
-        <v>67</v>
+        <v>73.40000000000001</v>
       </c>
       <c r="G18">
-        <v>66.40000000000001</v>
+        <v>72.90000000000001</v>
       </c>
       <c r="H18">
-        <v>64.3</v>
+        <v>71.7</v>
       </c>
       <c r="I18">
-        <v>60.9</v>
+        <v>70</v>
       </c>
       <c r="J18">
-        <v>56.6</v>
+        <v>68</v>
       </c>
       <c r="K18">
-        <v>51.6</v>
+        <v>65.90000000000001</v>
       </c>
       <c r="L18">
-        <v>46.5</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1129,37 +1129,37 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>55.3</v>
+        <v>60.1</v>
       </c>
       <c r="C19">
-        <v>57.2</v>
+        <v>62.3</v>
       </c>
       <c r="D19">
-        <v>58.7</v>
+        <v>63.9</v>
       </c>
       <c r="E19">
-        <v>59.5</v>
+        <v>65.09999999999999</v>
       </c>
       <c r="F19">
-        <v>59.4</v>
+        <v>65.7</v>
       </c>
       <c r="G19">
-        <v>58.3</v>
+        <v>65.7</v>
       </c>
       <c r="H19">
-        <v>56.3</v>
+        <v>65.2</v>
       </c>
       <c r="I19">
-        <v>53.4</v>
+        <v>64.40000000000001</v>
       </c>
       <c r="J19">
-        <v>49.8</v>
+        <v>63.4</v>
       </c>
       <c r="K19">
-        <v>45.9</v>
+        <v>62.3</v>
       </c>
       <c r="L19">
-        <v>41.9</v>
+        <v>61.2</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1167,37 +1167,37 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>55.9</v>
+        <v>65.7</v>
       </c>
       <c r="C20">
-        <v>60.4</v>
+        <v>70.2</v>
       </c>
       <c r="D20">
-        <v>64.59999999999999</v>
+        <v>74.09999999999999</v>
       </c>
       <c r="E20">
-        <v>68.09999999999999</v>
+        <v>77.09999999999999</v>
       </c>
       <c r="F20">
-        <v>70.59999999999999</v>
+        <v>79.2</v>
       </c>
       <c r="G20">
-        <v>72</v>
+        <v>80.2</v>
       </c>
       <c r="H20">
-        <v>72</v>
+        <v>80.2</v>
       </c>
       <c r="I20">
-        <v>70.7</v>
+        <v>79.40000000000001</v>
       </c>
       <c r="J20">
-        <v>68.3</v>
+        <v>77.90000000000001</v>
       </c>
       <c r="K20">
-        <v>65</v>
+        <v>75.90000000000001</v>
       </c>
       <c r="L20">
-        <v>61.1</v>
+        <v>73.5</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1205,37 +1205,37 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>47.1</v>
+        <v>55.6</v>
       </c>
       <c r="C21">
-        <v>51.3</v>
+        <v>59.2</v>
       </c>
       <c r="D21">
-        <v>55.2</v>
+        <v>62.1</v>
       </c>
       <c r="E21">
-        <v>58.4</v>
+        <v>63.8</v>
       </c>
       <c r="F21">
-        <v>60.5</v>
+        <v>64.40000000000001</v>
       </c>
       <c r="G21">
-        <v>61.5</v>
+        <v>63.7</v>
       </c>
       <c r="H21">
-        <v>61.1</v>
+        <v>62</v>
       </c>
       <c r="I21">
         <v>59.3</v>
       </c>
       <c r="J21">
-        <v>56.3</v>
+        <v>55.9</v>
       </c>
       <c r="K21">
         <v>52.3</v>
       </c>
       <c r="L21">
-        <v>47.7</v>
+        <v>48.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>